<commit_message>
Release 1.0.1 -- See release_notes.luma in /version/ for details
</commit_message>
<xml_diff>
--- a/LUMA/tools/SizingGuide.xlsx
+++ b/LUMA/tools/SizingGuide.xlsx
@@ -5,11 +5,11 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Adrian\OneDrive\Documents\SourceTree Repos\2d-3d-lbm-c-new\LatBo\tools\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Adrian\Dropbox (Personal)\0. Work\3. LBM\C++ Projects\LUMA\LUMA\tools\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9372" tabRatio="573"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9372" tabRatio="573" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Archer" sheetId="11" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="317" uniqueCount="80">
   <si>
     <t>No of Nodes</t>
   </si>
@@ -206,6 +206,73 @@
   </si>
   <si>
     <t>3D Aerofoil Cases AR = 2</t>
+  </si>
+  <si>
+    <t>3D Car</t>
+  </si>
+  <si>
+    <t>refXstart3</t>
+  </si>
+  <si>
+    <t>refXend3</t>
+  </si>
+  <si>
+    <t>refYstart3</t>
+  </si>
+  <si>
+    <t>refYend3</t>
+  </si>
+  <si>
+    <t>refZstart3</t>
+  </si>
+  <si>
+    <t>refZend3</t>
+  </si>
+  <si>
+    <t>N3</t>
+  </si>
+  <si>
+    <t>M3</t>
+  </si>
+  <si>
+    <t>K3</t>
+  </si>
+  <si>
+    <t>refXstart4</t>
+  </si>
+  <si>
+    <t>refXend4</t>
+  </si>
+  <si>
+    <t>refYstart4</t>
+  </si>
+  <si>
+    <t>refYend4</t>
+  </si>
+  <si>
+    <t>refZstart4</t>
+  </si>
+  <si>
+    <t>refZend4</t>
+  </si>
+  <si>
+    <t>N4</t>
+  </si>
+  <si>
+    <t>K4</t>
+  </si>
+  <si>
+    <t>M4</t>
+  </si>
+  <si>
+    <t>Grids = 4</t>
+  </si>
+  <si>
+    <t>Total Car</t>
+  </si>
+  <si>
+    <t>Points 
+per L</t>
   </si>
 </sst>
 </file>
@@ -239,7 +306,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -261,6 +328,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -293,7 +366,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -322,6 +395,7 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="1" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -737,10 +811,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet4"/>
-  <dimension ref="A1:N43"/>
+  <dimension ref="A1:N61"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="L33" sqref="L33"/>
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="B29" sqref="B29:C29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -806,49 +880,49 @@
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="4">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="B2" s="4">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C2" s="4">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D2" s="5">
         <f t="shared" ref="D2:D16" si="0">E2/$B$19</f>
-        <v>1</v>
+        <v>0.33333333333333331</v>
       </c>
       <c r="E2" s="5">
         <f t="shared" ref="E2:E16" si="1">A2*B2*C2</f>
-        <v>24</v>
+        <v>8</v>
       </c>
       <c r="F2" s="5">
         <f t="shared" ref="F2:F16" si="2">($C$24/A2)+2</f>
-        <v>152</v>
+        <v>98</v>
       </c>
       <c r="G2" s="5">
         <f t="shared" ref="G2:G16" si="3">($C$25/B2)+2</f>
-        <v>152</v>
+        <v>50</v>
       </c>
       <c r="H2" s="5">
         <f t="shared" ref="H2:H16" si="4">($C$26/C2)+2</f>
-        <v>802</v>
+        <v>74</v>
       </c>
       <c r="I2" s="5">
         <f t="shared" ref="I2:I16" si="5">F2*G2*H2</f>
-        <v>18529408</v>
+        <v>362600</v>
       </c>
       <c r="J2" s="5">
         <f t="shared" ref="J2:J16" si="6">4*F2*G2+4*G2*H2+4*F2*H2</f>
-        <v>1067648</v>
+        <v>63408</v>
       </c>
       <c r="K2" s="5">
         <f t="shared" ref="K2:K16" si="7">J2*E2</f>
-        <v>25623552</v>
+        <v>507264</v>
       </c>
       <c r="L2" s="5">
         <f t="shared" ref="L2:L16" si="8">K2/$C$27*100</f>
-        <v>5.9313777777777776</v>
+        <v>19.111689814814813</v>
       </c>
       <c r="M2" s="6" t="b">
         <f>IF((F2-FLOOR(F2,1))=0,IF((G2-FLOOR(G2,1))=0,IF((H2-FLOOR(H2,1))=0,TRUE,FALSE),FALSE),FALSE)</f>
@@ -856,54 +930,54 @@
       </c>
       <c r="N2" s="6" t="b">
         <f>IF(($D2-FLOOR($D2,1))=0,TRUE,FALSE)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" s="4">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="B3" s="4">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="C3" s="4">
-        <v>20</v>
+        <v>6</v>
       </c>
       <c r="D3" s="5">
         <f t="shared" si="0"/>
-        <v>250</v>
+        <v>32</v>
       </c>
       <c r="E3" s="5">
         <f t="shared" si="1"/>
-        <v>6000</v>
+        <v>768</v>
       </c>
       <c r="F3" s="5">
         <f t="shared" si="2"/>
-        <v>62</v>
+        <v>14</v>
       </c>
       <c r="G3" s="5">
         <f t="shared" si="3"/>
-        <v>32</v>
+        <v>14</v>
       </c>
       <c r="H3" s="5">
         <f t="shared" si="4"/>
-        <v>42</v>
+        <v>26</v>
       </c>
       <c r="I3" s="5">
         <f t="shared" si="5"/>
-        <v>83328</v>
+        <v>5096</v>
       </c>
       <c r="J3" s="5">
         <f t="shared" si="6"/>
-        <v>23728</v>
+        <v>3696</v>
       </c>
       <c r="K3" s="5">
         <f t="shared" si="7"/>
-        <v>142368000</v>
+        <v>2838528</v>
       </c>
       <c r="L3" s="5">
         <f t="shared" si="8"/>
-        <v>32.955555555555556</v>
+        <v>106.94444444444444</v>
       </c>
       <c r="M3" s="6" t="b">
         <f>IF((F3-FLOOR(F3,1))=0,IF((G3-FLOOR(G3,1))=0,IF((H3-FLOOR(H3,1))=0,TRUE,FALSE),FALSE),FALSE)</f>
@@ -916,53 +990,53 @@
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" s="4">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="B4" s="4">
-        <v>15</v>
+        <v>5</v>
       </c>
       <c r="C4" s="4">
-        <v>16</v>
+        <v>6</v>
       </c>
       <c r="D4" s="5">
         <f t="shared" si="0"/>
-        <v>160</v>
+        <v>25</v>
       </c>
       <c r="E4" s="5">
         <f t="shared" si="1"/>
-        <v>3840</v>
+        <v>600</v>
       </c>
       <c r="F4" s="5">
         <f t="shared" si="2"/>
-        <v>77</v>
+        <v>11.6</v>
       </c>
       <c r="G4" s="5">
         <f t="shared" si="3"/>
-        <v>32</v>
+        <v>21.2</v>
       </c>
       <c r="H4" s="5">
         <f t="shared" si="4"/>
-        <v>52</v>
+        <v>26</v>
       </c>
       <c r="I4" s="5">
         <f t="shared" si="5"/>
-        <v>128128</v>
+        <v>6393.92</v>
       </c>
       <c r="J4" s="5">
         <f t="shared" si="6"/>
-        <v>32528</v>
+        <v>4394.8799999999992</v>
       </c>
       <c r="K4" s="5">
         <f t="shared" si="7"/>
-        <v>124907520</v>
+        <v>2636927.9999999995</v>
       </c>
       <c r="L4" s="5">
         <f t="shared" si="8"/>
-        <v>28.913777777777778</v>
+        <v>99.348958333333314</v>
       </c>
       <c r="M4" s="6" t="b">
         <f t="shared" ref="M4:M6" si="10">IF((F4-FLOOR(F4,1))=0,IF((G4-FLOOR(G4,1))=0,IF((H4-FLOOR(H4,1))=0,TRUE,FALSE),FALSE),FALSE)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N4" s="6" t="b">
         <f t="shared" si="9"/>
@@ -989,35 +1063,35 @@
       </c>
       <c r="F5" s="5">
         <f t="shared" si="2"/>
-        <v>102</v>
+        <v>18</v>
       </c>
       <c r="G5" s="5">
         <f t="shared" si="3"/>
-        <v>47</v>
+        <v>11.6</v>
       </c>
       <c r="H5" s="5">
         <f t="shared" si="4"/>
-        <v>802</v>
+        <v>146</v>
       </c>
       <c r="I5" s="5">
         <f t="shared" si="5"/>
-        <v>3844788</v>
+        <v>30484.799999999999</v>
       </c>
       <c r="J5" s="5">
         <f t="shared" si="6"/>
-        <v>497168</v>
+        <v>18121.599999999999</v>
       </c>
       <c r="K5" s="5">
         <f t="shared" si="7"/>
-        <v>59660160</v>
+        <v>2174592</v>
       </c>
       <c r="L5" s="5">
         <f t="shared" si="8"/>
-        <v>13.810222222222221</v>
+        <v>81.929976851851848</v>
       </c>
       <c r="M5" s="6" t="b">
         <f t="shared" si="10"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N5" s="6" t="b">
         <f t="shared" si="9"/>
@@ -1044,35 +1118,35 @@
       </c>
       <c r="F6" s="5">
         <f t="shared" si="2"/>
-        <v>102</v>
+        <v>18</v>
       </c>
       <c r="G6" s="5">
         <f t="shared" si="3"/>
-        <v>92</v>
+        <v>21.2</v>
       </c>
       <c r="H6" s="5">
         <f t="shared" si="4"/>
-        <v>102</v>
+        <v>20</v>
       </c>
       <c r="I6" s="5">
         <f t="shared" si="5"/>
-        <v>957168</v>
+        <v>7631.9999999999991</v>
       </c>
       <c r="J6" s="5">
         <f t="shared" si="6"/>
-        <v>116688</v>
+        <v>4662.3999999999996</v>
       </c>
       <c r="K6" s="5">
         <f t="shared" si="7"/>
-        <v>56010240</v>
+        <v>2237952</v>
       </c>
       <c r="L6" s="5">
         <f t="shared" si="8"/>
-        <v>12.965333333333334</v>
+        <v>84.317129629629633</v>
       </c>
       <c r="M6" s="6" t="b">
         <f t="shared" si="10"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N6" s="6" t="b">
         <f t="shared" si="9"/>
@@ -1099,31 +1173,31 @@
       </c>
       <c r="F7" s="5">
         <f t="shared" si="2"/>
-        <v>102</v>
+        <v>18</v>
       </c>
       <c r="G7" s="5">
         <f t="shared" si="3"/>
-        <v>39.5</v>
+        <v>10</v>
       </c>
       <c r="H7" s="5">
         <f t="shared" si="4"/>
-        <v>82</v>
+        <v>16.399999999999999</v>
       </c>
       <c r="I7" s="5">
         <f t="shared" si="5"/>
-        <v>330378</v>
+        <v>2951.9999999999995</v>
       </c>
       <c r="J7" s="5">
         <f t="shared" si="6"/>
-        <v>62528</v>
+        <v>2556.8000000000002</v>
       </c>
       <c r="K7" s="5">
         <f t="shared" si="7"/>
-        <v>90040320</v>
+        <v>3681792.0000000005</v>
       </c>
       <c r="L7" s="5">
         <f t="shared" si="8"/>
-        <v>20.842666666666666</v>
+        <v>138.7152777777778</v>
       </c>
       <c r="M7" s="6" t="b">
         <f>IF((F7-FLOOR(F7,1))=0,IF((G7-FLOOR(G7,1))=0,IF((H7-FLOOR(H7,1))=0,TRUE,FALSE),FALSE),FALSE)</f>
@@ -1154,35 +1228,35 @@
       </c>
       <c r="F8" s="5">
         <f t="shared" si="2"/>
-        <v>102</v>
+        <v>18</v>
       </c>
       <c r="G8" s="5">
         <f t="shared" si="3"/>
-        <v>47</v>
+        <v>11.6</v>
       </c>
       <c r="H8" s="5">
         <f t="shared" si="4"/>
-        <v>402</v>
+        <v>74</v>
       </c>
       <c r="I8" s="5">
         <f t="shared" si="5"/>
-        <v>1927188</v>
+        <v>15451.199999999999</v>
       </c>
       <c r="J8" s="5">
         <f t="shared" si="6"/>
-        <v>258768</v>
+        <v>9596.7999999999993</v>
       </c>
       <c r="K8" s="5">
         <f t="shared" si="7"/>
-        <v>62104320</v>
+        <v>2303232</v>
       </c>
       <c r="L8" s="5">
         <f t="shared" si="8"/>
-        <v>14.375999999999999</v>
+        <v>86.776620370370367</v>
       </c>
       <c r="M8" s="6" t="b">
         <f t="shared" ref="M8:M16" si="11">IF((F8-FLOOR(F8,1))=0,IF((G8-FLOOR(G8,1))=0,IF((H8-FLOOR(H8,1))=0,TRUE,FALSE),FALSE),FALSE)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N8" s="6" t="b">
         <f t="shared" si="9"/>
@@ -1209,35 +1283,35 @@
       </c>
       <c r="F9" s="5">
         <f t="shared" si="2"/>
-        <v>152</v>
+        <v>26</v>
       </c>
       <c r="G9" s="5">
         <f t="shared" si="3"/>
-        <v>92</v>
+        <v>21.2</v>
       </c>
       <c r="H9" s="5">
         <f t="shared" si="4"/>
-        <v>202</v>
+        <v>38</v>
       </c>
       <c r="I9" s="5">
         <f t="shared" si="5"/>
-        <v>2824768</v>
+        <v>20945.599999999999</v>
       </c>
       <c r="J9" s="5">
         <f t="shared" si="6"/>
-        <v>253088</v>
+        <v>9379.2000000000007</v>
       </c>
       <c r="K9" s="5">
         <f t="shared" si="7"/>
-        <v>40494080</v>
+        <v>1500672</v>
       </c>
       <c r="L9" s="5">
         <f t="shared" si="8"/>
-        <v>9.3736296296296295</v>
+        <v>56.539351851851848</v>
       </c>
       <c r="M9" s="6" t="b">
         <f t="shared" si="11"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N9" s="6" t="b">
         <f t="shared" si="9"/>
@@ -1264,31 +1338,31 @@
       </c>
       <c r="F10" s="5">
         <f t="shared" si="2"/>
-        <v>122</v>
+        <v>21.2</v>
       </c>
       <c r="G10" s="5">
         <f t="shared" si="3"/>
-        <v>114.5</v>
+        <v>26</v>
       </c>
       <c r="H10" s="5">
         <f t="shared" si="4"/>
-        <v>202</v>
+        <v>38</v>
       </c>
       <c r="I10" s="5">
         <f t="shared" si="5"/>
-        <v>2821738</v>
+        <v>20945.599999999999</v>
       </c>
       <c r="J10" s="5">
         <f t="shared" si="6"/>
-        <v>246968</v>
+        <v>9379.1999999999989</v>
       </c>
       <c r="K10" s="5">
         <f t="shared" si="7"/>
-        <v>39514880</v>
+        <v>1500671.9999999998</v>
       </c>
       <c r="L10" s="5">
         <f t="shared" si="8"/>
-        <v>9.146962962962963</v>
+        <v>56.539351851851841</v>
       </c>
       <c r="M10" s="6" t="b">
         <f t="shared" si="11"/>
@@ -1319,35 +1393,35 @@
       </c>
       <c r="F11" s="5">
         <f t="shared" si="2"/>
-        <v>77</v>
+        <v>14</v>
       </c>
       <c r="G11" s="5">
         <f t="shared" si="3"/>
-        <v>92</v>
+        <v>21.2</v>
       </c>
       <c r="H11" s="5">
         <f t="shared" si="4"/>
-        <v>402</v>
+        <v>74</v>
       </c>
       <c r="I11" s="5">
         <f t="shared" si="5"/>
-        <v>2847768</v>
+        <v>21963.200000000001</v>
       </c>
       <c r="J11" s="5">
         <f t="shared" si="6"/>
-        <v>300088</v>
+        <v>11606.4</v>
       </c>
       <c r="K11" s="5">
         <f t="shared" si="7"/>
-        <v>48014080</v>
+        <v>1857024</v>
       </c>
       <c r="L11" s="5">
         <f t="shared" si="8"/>
-        <v>11.11437037037037</v>
+        <v>69.965277777777786</v>
       </c>
       <c r="M11" s="6" t="b">
         <f t="shared" si="11"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N11" s="6" t="b">
         <f t="shared" si="9"/>
@@ -1374,35 +1448,35 @@
       </c>
       <c r="F12" s="5">
         <f t="shared" si="2"/>
-        <v>152</v>
+        <v>26</v>
       </c>
       <c r="G12" s="5">
         <f t="shared" si="3"/>
-        <v>58.25</v>
+        <v>14</v>
       </c>
       <c r="H12" s="5">
         <f t="shared" si="4"/>
-        <v>135.33333333333334</v>
+        <v>26</v>
       </c>
       <c r="I12" s="5">
         <f t="shared" si="5"/>
-        <v>1198241.3333333335</v>
+        <v>9464</v>
       </c>
       <c r="J12" s="5">
         <f t="shared" si="6"/>
-        <v>149231.33333333334</v>
+        <v>5616</v>
       </c>
       <c r="K12" s="5">
         <f t="shared" si="7"/>
-        <v>57304832</v>
+        <v>2156544</v>
       </c>
       <c r="L12" s="5">
         <f t="shared" si="8"/>
-        <v>13.265007407407408</v>
+        <v>81.25</v>
       </c>
       <c r="M12" s="6" t="b">
         <f t="shared" si="11"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N12" s="6" t="b">
         <f t="shared" si="9"/>
@@ -1429,35 +1503,35 @@
       </c>
       <c r="F13" s="5">
         <f t="shared" si="2"/>
-        <v>77</v>
+        <v>14</v>
       </c>
       <c r="G13" s="5">
         <f t="shared" si="3"/>
-        <v>114.5</v>
+        <v>26</v>
       </c>
       <c r="H13" s="5">
         <f t="shared" si="4"/>
-        <v>202</v>
+        <v>38</v>
       </c>
       <c r="I13" s="5">
         <f t="shared" si="5"/>
-        <v>1780933</v>
+        <v>13832</v>
       </c>
       <c r="J13" s="5">
         <f t="shared" si="6"/>
-        <v>189998</v>
+        <v>7536</v>
       </c>
       <c r="K13" s="5">
         <f t="shared" si="7"/>
-        <v>48639488</v>
+        <v>1929216</v>
       </c>
       <c r="L13" s="5">
         <f t="shared" si="8"/>
-        <v>11.25914074074074</v>
+        <v>72.68518518518519</v>
       </c>
       <c r="M13" s="6" t="b">
         <f t="shared" si="11"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N13" s="6" t="b">
         <f t="shared" si="9"/>
@@ -1484,35 +1558,35 @@
       </c>
       <c r="F14" s="5">
         <f t="shared" si="2"/>
-        <v>152</v>
+        <v>26</v>
       </c>
       <c r="G14" s="5">
         <f t="shared" si="3"/>
-        <v>58.25</v>
+        <v>14</v>
       </c>
       <c r="H14" s="5">
         <f t="shared" si="4"/>
-        <v>202</v>
+        <v>38</v>
       </c>
       <c r="I14" s="5">
         <f t="shared" si="5"/>
-        <v>1788508</v>
+        <v>13832</v>
       </c>
       <c r="J14" s="5">
         <f t="shared" si="6"/>
-        <v>205298</v>
+        <v>7536</v>
       </c>
       <c r="K14" s="5">
         <f t="shared" si="7"/>
-        <v>52556288</v>
+        <v>1929216</v>
       </c>
       <c r="L14" s="5">
         <f t="shared" si="8"/>
-        <v>12.165807407407407</v>
+        <v>72.68518518518519</v>
       </c>
       <c r="M14" s="6" t="b">
         <f t="shared" si="11"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N14" s="6" t="b">
         <f t="shared" si="9"/>
@@ -1539,35 +1613,35 @@
       </c>
       <c r="F15" s="5">
         <f t="shared" si="2"/>
-        <v>77</v>
+        <v>14</v>
       </c>
       <c r="G15" s="5">
         <f t="shared" si="3"/>
-        <v>47</v>
+        <v>11.6</v>
       </c>
       <c r="H15" s="5">
         <f t="shared" si="4"/>
-        <v>402</v>
+        <v>74</v>
       </c>
       <c r="I15" s="5">
         <f t="shared" si="5"/>
-        <v>1454838</v>
+        <v>12017.6</v>
       </c>
       <c r="J15" s="5">
         <f t="shared" si="6"/>
-        <v>213868</v>
+        <v>8227.2000000000007</v>
       </c>
       <c r="K15" s="5">
         <f t="shared" si="7"/>
-        <v>68437760</v>
+        <v>2632704</v>
       </c>
       <c r="L15" s="5">
         <f t="shared" si="8"/>
-        <v>15.842074074074075</v>
+        <v>99.18981481481481</v>
       </c>
       <c r="M15" s="6" t="b">
         <f t="shared" si="11"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N15" s="6" t="b">
         <f t="shared" si="9"/>
@@ -1594,31 +1668,31 @@
       </c>
       <c r="F16" s="5">
         <f t="shared" si="2"/>
-        <v>122</v>
+        <v>21.2</v>
       </c>
       <c r="G16" s="5">
         <f t="shared" si="3"/>
-        <v>58.25</v>
+        <v>14</v>
       </c>
       <c r="H16" s="5">
         <f t="shared" si="4"/>
-        <v>202</v>
+        <v>38</v>
       </c>
       <c r="I16" s="5">
         <f t="shared" si="5"/>
-        <v>1435513</v>
+        <v>11278.4</v>
       </c>
       <c r="J16" s="5">
         <f t="shared" si="6"/>
-        <v>174068</v>
+        <v>6537.6</v>
       </c>
       <c r="K16" s="5">
         <f t="shared" si="7"/>
-        <v>55701760</v>
+        <v>2092032</v>
       </c>
       <c r="L16" s="5">
         <f t="shared" si="8"/>
-        <v>12.893925925925926</v>
+        <v>78.819444444444443</v>
       </c>
       <c r="M16" s="6" t="b">
         <f t="shared" si="11"/>
@@ -1629,7 +1703,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:11" ht="26.4" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:14" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A19" s="11" t="s">
         <v>9</v>
       </c>
@@ -1640,12 +1714,12 @@
         <v>23</v>
       </c>
     </row>
-    <row r="20" spans="1:11" ht="26.4" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:14" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
-        <v>10</v>
+        <v>79</v>
       </c>
       <c r="B20" s="14">
-        <v>100</v>
+        <v>24</v>
       </c>
       <c r="D20" s="10" t="s">
         <v>18</v>
@@ -1653,13 +1727,16 @@
       <c r="F20" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="M20" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>34</v>
       </c>
       <c r="B21" s="14">
-        <v>30</v>
+        <v>0</v>
       </c>
       <c r="F21" t="s">
         <v>25</v>
@@ -1670,31 +1747,41 @@
       <c r="J21" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="M21" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
       <c r="F22" t="s">
         <v>26</v>
       </c>
       <c r="G22" s="13">
         <f>0.5*($C$24-$B$20*COS($B$21*PI()/180))</f>
-        <v>556.6987298107781</v>
+        <v>84</v>
       </c>
       <c r="H22" t="s">
         <v>29</v>
       </c>
       <c r="I22" s="13">
         <f>$C$24/4</f>
-        <v>300</v>
+        <v>48</v>
       </c>
       <c r="J22" t="s">
         <v>38</v>
       </c>
       <c r="K22" s="13">
         <f>$C$24/4</f>
-        <v>300</v>
-      </c>
-    </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+        <v>48</v>
+      </c>
+      <c r="M22" t="s">
+        <v>38</v>
+      </c>
+      <c r="N22" s="16">
+        <f>0.25*(B24-4)*B20</f>
+        <v>24</v>
+      </c>
+    </row>
+    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A23" s="1"/>
       <c r="B23" s="1" t="s">
         <v>11</v>
@@ -1707,33 +1794,40 @@
       </c>
       <c r="G23" s="13">
         <f>0.5*($C$24-$B$20*SIN($B$21*PI()/180))</f>
-        <v>575</v>
+        <v>96</v>
       </c>
       <c r="H23" t="s">
         <v>30</v>
       </c>
       <c r="I23" s="13">
         <f>3*$C$24/4</f>
-        <v>900</v>
+        <v>144</v>
       </c>
       <c r="J23" t="s">
         <v>41</v>
       </c>
       <c r="K23" s="13">
         <f>3*$C$24/4</f>
-        <v>900</v>
-      </c>
-    </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+        <v>144</v>
+      </c>
+      <c r="M23" t="s">
+        <v>41</v>
+      </c>
+      <c r="N23" s="16">
+        <f>N22+(4*B20)</f>
+        <v>120</v>
+      </c>
+    </row>
+    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>4</v>
       </c>
       <c r="B24" s="15">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="C24" s="3">
         <f>$B$20*B24</f>
-        <v>1200</v>
+        <v>192</v>
       </c>
       <c r="E24" s="12"/>
       <c r="F24" t="s">
@@ -1741,33 +1835,39 @@
       </c>
       <c r="G24" s="13">
         <f>C26/2</f>
-        <v>400</v>
+        <v>72</v>
       </c>
       <c r="H24" s="12" t="s">
         <v>31</v>
       </c>
       <c r="I24" s="13">
         <f>$C$25/4</f>
-        <v>112.5</v>
+        <v>24</v>
       </c>
       <c r="J24" s="12" t="s">
         <v>40</v>
       </c>
       <c r="K24" s="13">
         <f>$C$25/4</f>
-        <v>112.5</v>
-      </c>
-    </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+        <v>24</v>
+      </c>
+      <c r="M24" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="N24" s="16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B25" s="15">
-        <v>4.5</v>
+        <v>4</v>
       </c>
       <c r="C25" s="3">
         <f t="shared" ref="C25" si="12">$B$20*B25</f>
-        <v>450</v>
+        <v>96</v>
       </c>
       <c r="E25" s="12"/>
       <c r="F25" t="s">
@@ -1775,264 +1875,562 @@
       </c>
       <c r="G25" s="12">
         <f>B20*COS(B21*PI()/180)</f>
-        <v>86.602540378443877</v>
+        <v>24</v>
       </c>
       <c r="H25" s="12" t="s">
         <v>32</v>
       </c>
       <c r="I25" s="13">
         <f>3*$C$25/4</f>
-        <v>337.5</v>
+        <v>72</v>
       </c>
       <c r="J25" s="12" t="s">
         <v>42</v>
       </c>
       <c r="K25" s="13">
         <f>3*$C$25/4</f>
-        <v>337.5</v>
-      </c>
-    </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+        <v>72</v>
+      </c>
+      <c r="M25" s="12" t="s">
+        <v>42</v>
+      </c>
+      <c r="N25" s="16">
+        <f>1.5*B20</f>
+        <v>36</v>
+      </c>
+    </row>
+    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>6</v>
       </c>
       <c r="B26" s="15">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C26" s="3">
         <f>IF(B26=0,1,$B$20*B26)</f>
-        <v>800</v>
+        <v>144</v>
       </c>
       <c r="H26" s="12" t="s">
         <v>49</v>
       </c>
       <c r="I26">
         <f>(($B$26-6)/2)*$B$20</f>
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="J26" s="12" t="s">
         <v>51</v>
       </c>
       <c r="K26">
         <f>(($B$26-6)/2)*$B$20</f>
-        <v>100</v>
-      </c>
-    </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+      <c r="M26" s="12" t="s">
+        <v>51</v>
+      </c>
+      <c r="N26" s="16">
+        <f>(B26/2-1.5)*B20</f>
+        <v>36</v>
+      </c>
+    </row>
+    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B27" s="1" t="s">
         <v>13</v>
       </c>
       <c r="C27" s="3">
         <f>C24*C25*C26</f>
-        <v>432000000</v>
+        <v>2654208</v>
       </c>
       <c r="H27" s="12" t="s">
         <v>50</v>
       </c>
       <c r="I27">
         <f>$I$26+6*$B$20</f>
-        <v>700</v>
+        <v>144</v>
       </c>
       <c r="J27" s="12" t="s">
         <v>52</v>
       </c>
       <c r="K27">
         <f>$I$26+6*$B$20</f>
-        <v>700</v>
-      </c>
-    </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+        <v>144</v>
+      </c>
+      <c r="M27" s="12" t="s">
+        <v>52</v>
+      </c>
+      <c r="N27" s="16">
+        <f>N26+(3*B20)</f>
+        <v>108</v>
+      </c>
+    </row>
+    <row r="28" spans="1:14" x14ac:dyDescent="0.25">
       <c r="H28" t="s">
         <v>35</v>
       </c>
       <c r="I28" s="13">
         <f>($I$23-$I$22+1)*2</f>
-        <v>1202</v>
+        <v>194</v>
       </c>
       <c r="J28" t="s">
         <v>35</v>
       </c>
       <c r="K28" s="13">
         <f>($I$23-$I$22+1)*2</f>
-        <v>1202</v>
-      </c>
-    </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+        <v>194</v>
+      </c>
+      <c r="M28" t="s">
+        <v>35</v>
+      </c>
+      <c r="N28" s="12">
+        <f>(N23-N22+1)*2</f>
+        <v>194</v>
+      </c>
+    </row>
+    <row r="29" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B29" t="s">
+        <v>78</v>
+      </c>
+      <c r="C29" s="13">
+        <f>(C24*C25*C26)+ (N28*N29*N30) + (N37*N38*N39) + (N46*N47*N48) + (N55*N56*N57)</f>
+        <v>163090688</v>
+      </c>
       <c r="H29" t="s">
         <v>36</v>
       </c>
       <c r="I29" s="13">
         <f>($I$25-$I$24+1)*2</f>
-        <v>452</v>
+        <v>98</v>
       </c>
       <c r="J29" t="s">
         <v>36</v>
       </c>
       <c r="K29" s="13">
         <f>($I$25-$I$24+1)*2</f>
-        <v>452</v>
-      </c>
-    </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
+        <v>98</v>
+      </c>
+      <c r="M29" t="s">
+        <v>36</v>
+      </c>
+      <c r="N29" s="12">
+        <f>(N25-N24+1)*2</f>
+        <v>74</v>
+      </c>
+    </row>
+    <row r="30" spans="1:14" x14ac:dyDescent="0.25">
       <c r="H30" s="12" t="s">
         <v>48</v>
       </c>
       <c r="I30" s="13">
         <f>($I$27-$I$26+1)*2</f>
-        <v>1202</v>
+        <v>290</v>
       </c>
       <c r="J30" s="12" t="s">
         <v>48</v>
       </c>
       <c r="K30">
         <f>($I$27-$I$26+1)*2</f>
-        <v>1202</v>
-      </c>
-    </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
+        <v>290</v>
+      </c>
+      <c r="M30" s="12" t="s">
+        <v>48</v>
+      </c>
+      <c r="N30" s="12">
+        <f>(N27-N26+1)*2</f>
+        <v>146</v>
+      </c>
+    </row>
+    <row r="31" spans="1:14" x14ac:dyDescent="0.25">
       <c r="H31" t="s">
         <v>26</v>
       </c>
       <c r="I31" s="13">
         <f>0.5*($I$28-$B$20*2*COS($B$21*PI()/180))</f>
-        <v>514.3974596215561</v>
+        <v>73</v>
       </c>
       <c r="J31" t="s">
         <v>43</v>
       </c>
       <c r="K31" s="13">
         <f>($K$28/4)</f>
-        <v>300.5</v>
-      </c>
-    </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
+        <v>48.5</v>
+      </c>
+      <c r="M31" t="s">
+        <v>43</v>
+      </c>
+      <c r="N31" s="16">
+        <f>(B20/4)*2</f>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="32" spans="1:14" x14ac:dyDescent="0.25">
       <c r="H32" s="12" t="s">
         <v>27</v>
       </c>
       <c r="I32" s="13">
         <f>0.5*($I$28-$B$20*2*SIN($B$21*PI()/180))</f>
-        <v>551</v>
+        <v>97</v>
       </c>
       <c r="J32" t="s">
         <v>39</v>
       </c>
       <c r="K32" s="13">
         <f>(3*$K$28/4)</f>
-        <v>901.5</v>
-      </c>
-    </row>
-    <row r="33" spans="8:11" x14ac:dyDescent="0.25">
+        <v>145.5</v>
+      </c>
+      <c r="M32" t="s">
+        <v>39</v>
+      </c>
+      <c r="N32" s="16">
+        <f>N31+(3.25*B20*2)</f>
+        <v>168</v>
+      </c>
+    </row>
+    <row r="33" spans="8:14" x14ac:dyDescent="0.25">
       <c r="H33" t="s">
         <v>56</v>
       </c>
       <c r="I33" s="13">
         <f>I30/2</f>
-        <v>601</v>
+        <v>145</v>
       </c>
       <c r="J33" s="12" t="s">
         <v>44</v>
       </c>
       <c r="K33" s="13">
         <f>($K$29/4)</f>
-        <v>113</v>
-      </c>
-    </row>
-    <row r="34" spans="8:11" x14ac:dyDescent="0.25">
+        <v>24.5</v>
+      </c>
+      <c r="M33" s="12" t="s">
+        <v>44</v>
+      </c>
+      <c r="N33" s="16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="8:14" x14ac:dyDescent="0.25">
       <c r="H34" s="12" t="s">
         <v>28</v>
       </c>
       <c r="I34" s="13">
         <f>$B$20*2*COS($B$21*PI()/180)</f>
-        <v>173.20508075688775</v>
+        <v>48</v>
       </c>
       <c r="J34" s="12" t="s">
         <v>45</v>
       </c>
       <c r="K34" s="13">
         <f>(3*$K$29/4)</f>
-        <v>339</v>
-      </c>
-    </row>
-    <row r="35" spans="8:11" x14ac:dyDescent="0.25">
+        <v>73.5</v>
+      </c>
+      <c r="M34" s="12" t="s">
+        <v>45</v>
+      </c>
+      <c r="N34" s="16">
+        <f>N33+(1.25*B20*2)</f>
+        <v>60</v>
+      </c>
+    </row>
+    <row r="35" spans="8:14" x14ac:dyDescent="0.25">
       <c r="H35" s="12"/>
       <c r="J35" s="12" t="s">
         <v>53</v>
       </c>
       <c r="K35">
         <f>$B$20*2</f>
-        <v>200</v>
-      </c>
-    </row>
-    <row r="36" spans="8:11" x14ac:dyDescent="0.25">
+        <v>48</v>
+      </c>
+      <c r="M35" s="12" t="s">
+        <v>53</v>
+      </c>
+      <c r="N35" s="16">
+        <f>(B20/4)*2</f>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="36" spans="8:14" x14ac:dyDescent="0.25">
       <c r="J36" s="12" t="s">
         <v>54</v>
       </c>
       <c r="K36">
         <f>K35+(5*B20*2)</f>
-        <v>1200</v>
-      </c>
-    </row>
-    <row r="37" spans="8:11" x14ac:dyDescent="0.25">
+        <v>288</v>
+      </c>
+      <c r="M36" s="12" t="s">
+        <v>54</v>
+      </c>
+      <c r="N36" s="16">
+        <f>N35+(2.5*B20*2)</f>
+        <v>132</v>
+      </c>
+    </row>
+    <row r="37" spans="8:14" x14ac:dyDescent="0.25">
       <c r="J37" t="s">
         <v>46</v>
       </c>
       <c r="K37" s="13">
         <f>($K$32-$K$31+1)*2</f>
-        <v>1204</v>
-      </c>
-    </row>
-    <row r="38" spans="8:11" x14ac:dyDescent="0.25">
+        <v>196</v>
+      </c>
+      <c r="M37" t="s">
+        <v>46</v>
+      </c>
+      <c r="N37" s="12">
+        <f>(N32-N31+1)*2</f>
+        <v>314</v>
+      </c>
+    </row>
+    <row r="38" spans="8:14" x14ac:dyDescent="0.25">
       <c r="J38" t="s">
         <v>47</v>
       </c>
       <c r="K38" s="13">
         <f>($K$34-$K$33+1)*2</f>
-        <v>454</v>
-      </c>
-    </row>
-    <row r="39" spans="8:11" x14ac:dyDescent="0.25">
+        <v>100</v>
+      </c>
+      <c r="M38" t="s">
+        <v>47</v>
+      </c>
+      <c r="N38" s="12">
+        <f>(N34-N33+1)*2</f>
+        <v>122</v>
+      </c>
+    </row>
+    <row r="39" spans="8:14" x14ac:dyDescent="0.25">
       <c r="J39" s="12" t="s">
         <v>55</v>
       </c>
       <c r="K39" s="13">
         <f>($K$36-$K$35+1)*2</f>
-        <v>2002</v>
-      </c>
-    </row>
-    <row r="40" spans="8:11" x14ac:dyDescent="0.25">
+        <v>482</v>
+      </c>
+      <c r="M39" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="N39" s="12">
+        <f>(N36-N35+1)*2</f>
+        <v>242</v>
+      </c>
+    </row>
+    <row r="40" spans="8:14" x14ac:dyDescent="0.25">
       <c r="J40" t="s">
         <v>26</v>
       </c>
       <c r="K40" s="13">
         <f>0.5*($K$37-$B$20*4*COS($B$21*PI()/180))</f>
-        <v>428.79491924311225</v>
-      </c>
-    </row>
-    <row r="41" spans="8:11" x14ac:dyDescent="0.25">
+        <v>50</v>
+      </c>
+      <c r="M40" t="s">
+        <v>59</v>
+      </c>
+      <c r="N40" s="16">
+        <f>(B20/4)*4</f>
+        <v>24</v>
+      </c>
+    </row>
+    <row r="41" spans="8:14" x14ac:dyDescent="0.25">
       <c r="J41" s="12" t="s">
         <v>27</v>
       </c>
       <c r="K41" s="13">
         <f>0.5*($K$38-$B$20*4*SIN($B$21*PI()/180))</f>
-        <v>127.00000000000001</v>
-      </c>
-    </row>
-    <row r="42" spans="8:11" x14ac:dyDescent="0.25">
+        <v>50</v>
+      </c>
+      <c r="M41" t="s">
+        <v>60</v>
+      </c>
+      <c r="N41" s="16">
+        <f>N40+(2.5*B20*4)</f>
+        <v>264</v>
+      </c>
+    </row>
+    <row r="42" spans="8:14" x14ac:dyDescent="0.25">
       <c r="J42" t="s">
         <v>56</v>
       </c>
       <c r="K42" s="13">
         <f>K39/2</f>
-        <v>1001</v>
-      </c>
-    </row>
-    <row r="43" spans="8:11" x14ac:dyDescent="0.25">
+        <v>241</v>
+      </c>
+      <c r="M42" s="12" t="s">
+        <v>61</v>
+      </c>
+      <c r="N42" s="16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="8:14" x14ac:dyDescent="0.25">
       <c r="J43" s="12" t="s">
         <v>28</v>
       </c>
       <c r="K43" s="13">
         <f>$B$20*4*COS($B$21*PI()/180)</f>
-        <v>346.41016151377551</v>
+        <v>96</v>
+      </c>
+      <c r="M43" s="12" t="s">
+        <v>62</v>
+      </c>
+      <c r="N43" s="16">
+        <f>B20*4</f>
+        <v>96</v>
+      </c>
+    </row>
+    <row r="44" spans="8:14" x14ac:dyDescent="0.25">
+      <c r="M44" s="12" t="s">
+        <v>63</v>
+      </c>
+      <c r="N44" s="16">
+        <f>(B20/4)*4</f>
+        <v>24</v>
+      </c>
+    </row>
+    <row r="45" spans="8:14" x14ac:dyDescent="0.25">
+      <c r="M45" s="12" t="s">
+        <v>64</v>
+      </c>
+      <c r="N45" s="16">
+        <f>N44+(2*B20*4)</f>
+        <v>216</v>
+      </c>
+    </row>
+    <row r="46" spans="8:14" x14ac:dyDescent="0.25">
+      <c r="M46" t="s">
+        <v>65</v>
+      </c>
+      <c r="N46" s="12">
+        <f>(N41-N40+1)*2</f>
+        <v>482</v>
+      </c>
+    </row>
+    <row r="47" spans="8:14" x14ac:dyDescent="0.25">
+      <c r="M47" t="s">
+        <v>66</v>
+      </c>
+      <c r="N47" s="12">
+        <f>(N43-N42+1)*2</f>
+        <v>194</v>
+      </c>
+    </row>
+    <row r="48" spans="8:14" x14ac:dyDescent="0.25">
+      <c r="M48" s="12" t="s">
+        <v>67</v>
+      </c>
+      <c r="N48" s="12">
+        <f>(N45-N44+1)*2</f>
+        <v>386</v>
+      </c>
+    </row>
+    <row r="49" spans="13:14" x14ac:dyDescent="0.25">
+      <c r="M49" t="s">
+        <v>68</v>
+      </c>
+      <c r="N49" s="16">
+        <f>(B20/4)*8</f>
+        <v>48</v>
+      </c>
+    </row>
+    <row r="50" spans="13:14" x14ac:dyDescent="0.25">
+      <c r="M50" t="s">
+        <v>69</v>
+      </c>
+      <c r="N50" s="16">
+        <f>N49+(1.75*B20*8)</f>
+        <v>384</v>
+      </c>
+    </row>
+    <row r="51" spans="13:14" x14ac:dyDescent="0.25">
+      <c r="M51" s="12" t="s">
+        <v>70</v>
+      </c>
+      <c r="N51" s="16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="13:14" x14ac:dyDescent="0.25">
+      <c r="M52" s="12" t="s">
+        <v>71</v>
+      </c>
+      <c r="N52" s="16">
+        <f>0.75*B20*8</f>
+        <v>144</v>
+      </c>
+    </row>
+    <row r="53" spans="13:14" x14ac:dyDescent="0.25">
+      <c r="M53" s="12" t="s">
+        <v>72</v>
+      </c>
+      <c r="N53" s="16">
+        <f>(B20/4)*8</f>
+        <v>48</v>
+      </c>
+    </row>
+    <row r="54" spans="13:14" x14ac:dyDescent="0.25">
+      <c r="M54" s="12" t="s">
+        <v>73</v>
+      </c>
+      <c r="N54" s="16">
+        <f>N53+(1.5*B20*8)</f>
+        <v>336</v>
+      </c>
+    </row>
+    <row r="55" spans="13:14" x14ac:dyDescent="0.25">
+      <c r="M55" t="s">
+        <v>74</v>
+      </c>
+      <c r="N55" s="12">
+        <f>(N50-N49+1)*2</f>
+        <v>674</v>
+      </c>
+    </row>
+    <row r="56" spans="13:14" x14ac:dyDescent="0.25">
+      <c r="M56" t="s">
+        <v>76</v>
+      </c>
+      <c r="N56" s="12">
+        <f>(N52-N51+1)*2</f>
+        <v>290</v>
+      </c>
+    </row>
+    <row r="57" spans="13:14" x14ac:dyDescent="0.25">
+      <c r="M57" s="12" t="s">
+        <v>75</v>
+      </c>
+      <c r="N57" s="12">
+        <f>(N54-N53+1)*2</f>
+        <v>578</v>
+      </c>
+    </row>
+    <row r="58" spans="13:14" x14ac:dyDescent="0.25">
+      <c r="M58" t="s">
+        <v>26</v>
+      </c>
+      <c r="N58" s="16">
+        <f>(B20/4)*16</f>
+        <v>96</v>
+      </c>
+    </row>
+    <row r="59" spans="13:14" x14ac:dyDescent="0.25">
+      <c r="M59" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="N59" s="16">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="60" spans="13:14" x14ac:dyDescent="0.25">
+      <c r="M60" t="s">
+        <v>56</v>
+      </c>
+      <c r="N60" s="16">
+        <f>N57/2</f>
+        <v>289</v>
+      </c>
+    </row>
+    <row r="61" spans="13:14" x14ac:dyDescent="0.25">
+      <c r="M61" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="N61" s="16">
+        <f>B20*16</f>
+        <v>384</v>
       </c>
     </row>
   </sheetData>
@@ -2045,7 +2443,7 @@
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
-  <pageSetup paperSize="9" orientation="portrait" useFirstPageNumber="1" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" useFirstPageNumber="1" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>
   <headerFooter>
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
@@ -2056,10 +2454,10 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:N34"/>
+  <dimension ref="A1:N61"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="E32" sqref="E32"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -2143,35 +2541,35 @@
       </c>
       <c r="F2" s="5">
         <f t="shared" ref="F2:F16" si="2">($C$24/A2)+2</f>
-        <v>189.5</v>
+        <v>7</v>
       </c>
       <c r="G2" s="5">
         <f t="shared" ref="G2:G16" si="3">($C$25/B2)+2</f>
-        <v>152</v>
+        <v>7</v>
       </c>
       <c r="H2" s="5">
         <f t="shared" ref="H2:H16" si="4">($C$26/C2)+2</f>
-        <v>302</v>
+        <v>17</v>
       </c>
       <c r="I2" s="5">
         <f t="shared" ref="I2:I16" si="5">F2*G2*H2</f>
-        <v>8698808</v>
+        <v>833</v>
       </c>
       <c r="J2" s="5">
         <f t="shared" ref="J2:J16" si="6">4*F2*G2+4*G2*H2+4*F2*H2</f>
-        <v>527748</v>
+        <v>1148</v>
       </c>
       <c r="K2" s="5">
         <f t="shared" ref="K2:K16" si="7">J2*E2</f>
-        <v>33775872</v>
+        <v>73472</v>
       </c>
       <c r="L2" s="5">
         <f t="shared" ref="L2:L16" si="8">K2/$C$27*100</f>
-        <v>6.2547911111111114</v>
+        <v>306.13333333333333</v>
       </c>
       <c r="M2" s="6" t="b">
         <f>IF((F2-FLOOR(F2,1))=0,IF((G2-FLOOR(G2,1))=0,IF((H2-FLOOR(H2,1))=0,TRUE,FALSE),FALSE),FALSE)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N2" s="6" t="b">
         <f>IF(($D2-FLOOR($D2,1))=0,TRUE,FALSE)</f>
@@ -2198,31 +2596,31 @@
       </c>
       <c r="F3" s="5">
         <f t="shared" si="2"/>
-        <v>189.5</v>
+        <v>7</v>
       </c>
       <c r="G3" s="5">
         <f t="shared" si="3"/>
-        <v>152</v>
+        <v>7</v>
       </c>
       <c r="H3" s="5">
         <f t="shared" si="4"/>
-        <v>152</v>
+        <v>9.5</v>
       </c>
       <c r="I3" s="5">
         <f t="shared" si="5"/>
-        <v>4378208</v>
+        <v>465.5</v>
       </c>
       <c r="J3" s="5">
         <f t="shared" si="6"/>
-        <v>322848</v>
+        <v>728</v>
       </c>
       <c r="K3" s="5">
         <f t="shared" si="7"/>
-        <v>41324544</v>
+        <v>93184</v>
       </c>
       <c r="L3" s="5">
         <f t="shared" si="8"/>
-        <v>7.6526933333333336</v>
+        <v>388.26666666666665</v>
       </c>
       <c r="M3" s="6" t="b">
         <f>IF((F3-FLOOR(F3,1))=0,IF((G3-FLOOR(G3,1))=0,IF((H3-FLOOR(H3,1))=0,TRUE,FALSE),FALSE),FALSE)</f>
@@ -2253,35 +2651,35 @@
       </c>
       <c r="F4" s="5">
         <f t="shared" si="2"/>
-        <v>127</v>
+        <v>5.3333333333333339</v>
       </c>
       <c r="G4" s="5">
         <f t="shared" si="3"/>
-        <v>152</v>
+        <v>7</v>
       </c>
       <c r="H4" s="5">
         <f t="shared" si="4"/>
-        <v>152</v>
+        <v>9.5</v>
       </c>
       <c r="I4" s="5">
         <f t="shared" si="5"/>
-        <v>2934208</v>
+        <v>354.66666666666669</v>
       </c>
       <c r="J4" s="5">
         <f t="shared" si="6"/>
-        <v>246848</v>
+        <v>618</v>
       </c>
       <c r="K4" s="5">
         <f t="shared" si="7"/>
-        <v>47394816</v>
+        <v>118656</v>
       </c>
       <c r="L4" s="5">
         <f t="shared" si="8"/>
-        <v>8.7768177777777776</v>
+        <v>494.4</v>
       </c>
       <c r="M4" s="6" t="b">
         <f t="shared" ref="M4:M6" si="10">IF((F4-FLOOR(F4,1))=0,IF((G4-FLOOR(G4,1))=0,IF((H4-FLOOR(H4,1))=0,TRUE,FALSE),FALSE),FALSE)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N4" s="6" t="b">
         <f t="shared" si="9"/>
@@ -2290,53 +2688,53 @@
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" s="4">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="B5" s="4">
         <v>4</v>
       </c>
       <c r="C5" s="4">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="D5" s="5">
         <f t="shared" si="0"/>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E5" s="5">
         <f t="shared" si="1"/>
-        <v>256</v>
+        <v>192</v>
       </c>
       <c r="F5" s="5">
         <f t="shared" si="2"/>
-        <v>95.75</v>
+        <v>7</v>
       </c>
       <c r="G5" s="5">
         <f t="shared" si="3"/>
-        <v>152</v>
+        <v>7</v>
       </c>
       <c r="H5" s="5">
         <f t="shared" si="4"/>
-        <v>152</v>
+        <v>7</v>
       </c>
       <c r="I5" s="5">
         <f t="shared" si="5"/>
-        <v>2212208</v>
+        <v>343</v>
       </c>
       <c r="J5" s="5">
         <f t="shared" si="6"/>
-        <v>208848</v>
+        <v>588</v>
       </c>
       <c r="K5" s="5">
         <f t="shared" si="7"/>
-        <v>53465088</v>
+        <v>112896</v>
       </c>
       <c r="L5" s="5">
         <f t="shared" si="8"/>
-        <v>9.9009422222222234</v>
+        <v>470.4</v>
       </c>
       <c r="M5" s="6" t="b">
         <f t="shared" si="10"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N5" s="6" t="b">
         <f t="shared" si="9"/>
@@ -2363,35 +2761,35 @@
       </c>
       <c r="F6" s="5">
         <f t="shared" si="2"/>
-        <v>77</v>
+        <v>4</v>
       </c>
       <c r="G6" s="5">
         <f t="shared" si="3"/>
-        <v>152</v>
+        <v>7</v>
       </c>
       <c r="H6" s="5">
         <f t="shared" si="4"/>
-        <v>152</v>
+        <v>9.5</v>
       </c>
       <c r="I6" s="5">
         <f t="shared" si="5"/>
-        <v>1779008</v>
+        <v>266</v>
       </c>
       <c r="J6" s="5">
         <f t="shared" si="6"/>
-        <v>186048</v>
+        <v>530</v>
       </c>
       <c r="K6" s="5">
         <f t="shared" si="7"/>
-        <v>59535360</v>
+        <v>169600</v>
       </c>
       <c r="L6" s="5">
         <f t="shared" si="8"/>
-        <v>11.025066666666666</v>
+        <v>706.66666666666663</v>
       </c>
       <c r="M6" s="6" t="b">
         <f t="shared" si="10"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N6" s="6" t="b">
         <f t="shared" si="9"/>
@@ -2418,31 +2816,31 @@
       </c>
       <c r="F7" s="5">
         <f t="shared" si="2"/>
-        <v>377</v>
+        <v>12</v>
       </c>
       <c r="G7" s="5">
         <f t="shared" si="3"/>
-        <v>68.666666666666671</v>
+        <v>4.2222222222222223</v>
       </c>
       <c r="H7" s="5">
         <f t="shared" si="4"/>
-        <v>152</v>
+        <v>9.5</v>
       </c>
       <c r="I7" s="5">
         <f t="shared" si="5"/>
-        <v>3934874.666666667</v>
+        <v>481.33333333333337</v>
       </c>
       <c r="J7" s="5">
         <f t="shared" si="6"/>
-        <v>374514.66666666669</v>
+        <v>819.11111111111109</v>
       </c>
       <c r="K7" s="5">
         <f t="shared" si="7"/>
-        <v>53930112</v>
+        <v>117952</v>
       </c>
       <c r="L7" s="5">
         <f t="shared" si="8"/>
-        <v>9.9870577777777783</v>
+        <v>491.46666666666664</v>
       </c>
       <c r="M7" s="6" t="b">
         <f>IF((F7-FLOOR(F7,1))=0,IF((G7-FLOOR(G7,1))=0,IF((H7-FLOOR(H7,1))=0,TRUE,FALSE),FALSE),FALSE)</f>
@@ -2473,31 +2871,31 @@
       </c>
       <c r="F8" s="5">
         <f t="shared" si="2"/>
-        <v>189.5</v>
+        <v>7</v>
       </c>
       <c r="G8" s="5">
         <f t="shared" si="3"/>
-        <v>77</v>
+        <v>4.5</v>
       </c>
       <c r="H8" s="5">
         <f t="shared" si="4"/>
-        <v>602</v>
+        <v>32</v>
       </c>
       <c r="I8" s="5">
         <f t="shared" si="5"/>
-        <v>8784083</v>
+        <v>1008</v>
       </c>
       <c r="J8" s="5">
         <f t="shared" si="6"/>
-        <v>700098</v>
+        <v>1598</v>
       </c>
       <c r="K8" s="5">
         <f t="shared" si="7"/>
-        <v>44806272</v>
+        <v>102272</v>
       </c>
       <c r="L8" s="5">
         <f t="shared" si="8"/>
-        <v>8.2974577777777778</v>
+        <v>426.13333333333333</v>
       </c>
       <c r="M8" s="6" t="b">
         <f t="shared" ref="M8:M16" si="11">IF((F8-FLOOR(F8,1))=0,IF((G8-FLOOR(G8,1))=0,IF((H8-FLOOR(H8,1))=0,TRUE,FALSE),FALSE),FALSE)</f>
@@ -2528,31 +2926,31 @@
       </c>
       <c r="F9" s="5">
         <f t="shared" si="2"/>
-        <v>95.75</v>
+        <v>4.5</v>
       </c>
       <c r="G9" s="5">
         <f t="shared" si="3"/>
-        <v>77</v>
+        <v>4.5</v>
       </c>
       <c r="H9" s="5">
         <f t="shared" si="4"/>
-        <v>602</v>
+        <v>32</v>
       </c>
       <c r="I9" s="5">
         <f t="shared" si="5"/>
-        <v>4438395.5</v>
+        <v>648</v>
       </c>
       <c r="J9" s="5">
         <f t="shared" si="6"/>
-        <v>445473</v>
+        <v>1233</v>
       </c>
       <c r="K9" s="5">
         <f t="shared" si="7"/>
-        <v>57020544</v>
+        <v>157824</v>
       </c>
       <c r="L9" s="5">
         <f t="shared" si="8"/>
-        <v>10.55936</v>
+        <v>657.59999999999991</v>
       </c>
       <c r="M9" s="6" t="b">
         <f t="shared" si="11"/>
@@ -2583,31 +2981,31 @@
       </c>
       <c r="F10" s="5">
         <f t="shared" si="2"/>
-        <v>64.5</v>
+        <v>3.666666666666667</v>
       </c>
       <c r="G10" s="5">
         <f t="shared" si="3"/>
-        <v>77</v>
+        <v>4.5</v>
       </c>
       <c r="H10" s="5">
         <f t="shared" si="4"/>
-        <v>602</v>
+        <v>32</v>
       </c>
       <c r="I10" s="5">
         <f t="shared" si="5"/>
-        <v>2989833</v>
+        <v>528</v>
       </c>
       <c r="J10" s="5">
         <f t="shared" si="6"/>
-        <v>360598</v>
+        <v>1111.3333333333335</v>
       </c>
       <c r="K10" s="5">
         <f t="shared" si="7"/>
-        <v>69234816</v>
+        <v>213376.00000000003</v>
       </c>
       <c r="L10" s="5">
         <f t="shared" si="8"/>
-        <v>12.821262222222222</v>
+        <v>889.06666666666683</v>
       </c>
       <c r="M10" s="6" t="b">
         <f t="shared" si="11"/>
@@ -2638,31 +3036,31 @@
       </c>
       <c r="F11" s="5">
         <f t="shared" si="2"/>
-        <v>48.875</v>
+        <v>3.25</v>
       </c>
       <c r="G11" s="5">
         <f t="shared" si="3"/>
-        <v>77</v>
+        <v>4.5</v>
       </c>
       <c r="H11" s="5">
         <f t="shared" si="4"/>
-        <v>602</v>
+        <v>32</v>
       </c>
       <c r="I11" s="5">
         <f t="shared" si="5"/>
-        <v>2265551.75</v>
+        <v>468</v>
       </c>
       <c r="J11" s="5">
         <f t="shared" si="6"/>
-        <v>318160.5</v>
+        <v>1050.5</v>
       </c>
       <c r="K11" s="5">
         <f t="shared" si="7"/>
-        <v>81449088</v>
+        <v>268928</v>
       </c>
       <c r="L11" s="5">
         <f t="shared" si="8"/>
-        <v>15.083164444444444</v>
+        <v>1120.5333333333333</v>
       </c>
       <c r="M11" s="6" t="b">
         <f t="shared" si="11"/>
@@ -2693,31 +3091,31 @@
       </c>
       <c r="F12" s="5">
         <f t="shared" si="2"/>
-        <v>39.5</v>
+        <v>3</v>
       </c>
       <c r="G12" s="5">
         <f t="shared" si="3"/>
-        <v>77</v>
+        <v>4.5</v>
       </c>
       <c r="H12" s="5">
         <f t="shared" si="4"/>
-        <v>602</v>
+        <v>32</v>
       </c>
       <c r="I12" s="5">
         <f t="shared" si="5"/>
-        <v>1830983</v>
+        <v>432</v>
       </c>
       <c r="J12" s="5">
         <f t="shared" si="6"/>
-        <v>292698</v>
+        <v>1014</v>
       </c>
       <c r="K12" s="5">
         <f t="shared" si="7"/>
-        <v>93663360</v>
+        <v>324480</v>
       </c>
       <c r="L12" s="5">
         <f t="shared" si="8"/>
-        <v>17.345066666666668</v>
+        <v>1352</v>
       </c>
       <c r="M12" s="6" t="b">
         <f t="shared" si="11"/>
@@ -2748,31 +3146,31 @@
       </c>
       <c r="F13" s="5">
         <f t="shared" si="2"/>
-        <v>95.75</v>
+        <v>4.5</v>
       </c>
       <c r="G13" s="5">
         <f t="shared" si="3"/>
-        <v>68.666666666666671</v>
+        <v>4.2222222222222223</v>
       </c>
       <c r="H13" s="5">
         <f t="shared" si="4"/>
-        <v>152</v>
+        <v>9.5</v>
       </c>
       <c r="I13" s="5">
         <f t="shared" si="5"/>
-        <v>999374.66666666674</v>
+        <v>180.5</v>
       </c>
       <c r="J13" s="5">
         <f t="shared" si="6"/>
-        <v>126264.66666666667</v>
+        <v>407.44444444444446</v>
       </c>
       <c r="K13" s="5">
         <f t="shared" si="7"/>
-        <v>72728448</v>
+        <v>234688</v>
       </c>
       <c r="L13" s="5">
         <f t="shared" si="8"/>
-        <v>13.468231111111113</v>
+        <v>977.86666666666656</v>
       </c>
       <c r="M13" s="6" t="b">
         <f t="shared" si="11"/>
@@ -2803,31 +3201,31 @@
       </c>
       <c r="F14" s="5">
         <f t="shared" si="2"/>
-        <v>377</v>
+        <v>12</v>
       </c>
       <c r="G14" s="5">
         <f t="shared" si="3"/>
-        <v>302</v>
+        <v>12</v>
       </c>
       <c r="H14" s="5">
         <f t="shared" si="4"/>
-        <v>302</v>
+        <v>17</v>
       </c>
       <c r="I14" s="5">
         <f t="shared" si="5"/>
-        <v>34383908</v>
+        <v>2448</v>
       </c>
       <c r="J14" s="5">
         <f t="shared" si="6"/>
-        <v>1275648</v>
+        <v>2208</v>
       </c>
       <c r="K14" s="5">
         <f t="shared" si="7"/>
-        <v>20410368</v>
+        <v>35328</v>
       </c>
       <c r="L14" s="5">
         <f t="shared" si="8"/>
-        <v>3.7796977777777774</v>
+        <v>147.19999999999999</v>
       </c>
       <c r="M14" s="6" t="b">
         <f t="shared" si="11"/>
@@ -2858,31 +3256,31 @@
       </c>
       <c r="F15" s="5">
         <f t="shared" si="2"/>
-        <v>752</v>
+        <v>22</v>
       </c>
       <c r="G15" s="5">
         <f t="shared" si="3"/>
-        <v>302</v>
+        <v>12</v>
       </c>
       <c r="H15" s="5">
         <f t="shared" si="4"/>
-        <v>302</v>
+        <v>17</v>
       </c>
       <c r="I15" s="5">
         <f t="shared" si="5"/>
-        <v>68585408</v>
+        <v>4488</v>
       </c>
       <c r="J15" s="5">
         <f t="shared" si="6"/>
-        <v>2181648</v>
+        <v>3368</v>
       </c>
       <c r="K15" s="5">
         <f t="shared" si="7"/>
-        <v>17453184</v>
+        <v>26944</v>
       </c>
       <c r="L15" s="5">
         <f t="shared" si="8"/>
-        <v>3.2320711111111109</v>
+        <v>112.26666666666667</v>
       </c>
       <c r="M15" s="6" t="b">
         <f t="shared" si="11"/>
@@ -2913,42 +3311,42 @@
       </c>
       <c r="F16" s="5">
         <f t="shared" si="2"/>
-        <v>152</v>
+        <v>6</v>
       </c>
       <c r="G16" s="5">
         <f t="shared" si="3"/>
-        <v>77</v>
+        <v>4.5</v>
       </c>
       <c r="H16" s="5">
         <f t="shared" si="4"/>
-        <v>77</v>
+        <v>5.75</v>
       </c>
       <c r="I16" s="5">
         <f t="shared" si="5"/>
-        <v>901208</v>
+        <v>155.25</v>
       </c>
       <c r="J16" s="5">
         <f t="shared" si="6"/>
-        <v>117348</v>
+        <v>349.5</v>
       </c>
       <c r="K16" s="5">
         <f t="shared" si="7"/>
-        <v>75102720</v>
+        <v>223680</v>
       </c>
       <c r="L16" s="5">
         <f t="shared" si="8"/>
-        <v>13.90791111111111</v>
+        <v>932</v>
       </c>
       <c r="M16" s="6" t="b">
         <f t="shared" si="11"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N16" s="6" t="b">
         <f t="shared" si="9"/>
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:13" ht="26.4" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:14" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A19" s="11" t="s">
         <v>9</v>
       </c>
@@ -2959,18 +3357,35 @@
         <v>23</v>
       </c>
     </row>
-    <row r="20" spans="1:13" ht="26.4" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:14" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
         <v>10</v>
       </c>
       <c r="B20">
-        <v>150</v>
+        <v>5</v>
       </c>
       <c r="D20" s="10" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="M20" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="M21" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="M22" t="s">
+        <v>38</v>
+      </c>
+      <c r="N22" s="16">
+        <f>0.25*(B24-4)*B20</f>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A23" s="1"/>
       <c r="B23" s="1" t="s">
         <v>11</v>
@@ -2978,24 +3393,36 @@
       <c r="C23" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="M23" s="12"/>
-    </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="M23" t="s">
+        <v>41</v>
+      </c>
+      <c r="N23" s="16">
+        <f>N22+(4*B20)</f>
+        <v>25</v>
+      </c>
+    </row>
+    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>4</v>
       </c>
       <c r="B24" s="1">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C24" s="3">
         <f>$B$20*B24</f>
-        <v>1500</v>
+        <v>40</v>
       </c>
       <c r="E24" s="12"/>
       <c r="H24" s="12"/>
       <c r="J24" s="12"/>
-    </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="M24" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="N24" s="16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>5</v>
       </c>
@@ -3004,60 +3431,376 @@
       </c>
       <c r="C25" s="3">
         <f t="shared" ref="C25:C26" si="12">$B$20*B25</f>
-        <v>600</v>
+        <v>20</v>
       </c>
       <c r="E25" s="12"/>
       <c r="H25" s="12"/>
       <c r="J25" s="12"/>
-    </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="M25" s="12" t="s">
+        <v>42</v>
+      </c>
+      <c r="N25" s="16">
+        <f>1.5*B20</f>
+        <v>7.5</v>
+      </c>
+    </row>
+    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>6</v>
       </c>
       <c r="B26" s="1">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C26" s="3">
         <f t="shared" si="12"/>
-        <v>600</v>
+        <v>30</v>
       </c>
       <c r="J26" s="12"/>
-    </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="M26" s="12" t="s">
+        <v>51</v>
+      </c>
+      <c r="N26" s="16">
+        <f>((B26/2-1.5)*B20) - 1</f>
+        <v>6.5</v>
+      </c>
+    </row>
+    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B27" s="1" t="s">
         <v>13</v>
       </c>
       <c r="C27" s="3">
         <f>C24*C25*C26</f>
-        <v>540000000</v>
+        <v>24000</v>
       </c>
       <c r="H27" s="12"/>
       <c r="J27" s="12"/>
-    </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="M27" s="12" t="s">
+        <v>52</v>
+      </c>
+      <c r="N27" s="16">
+        <f>N26+(3*B20)</f>
+        <v>21.5</v>
+      </c>
+    </row>
+    <row r="28" spans="1:14" x14ac:dyDescent="0.25">
       <c r="H28" s="12"/>
       <c r="J28" s="12"/>
-    </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="M28" t="s">
+        <v>35</v>
+      </c>
+      <c r="N28" s="12">
+        <f>(N23-N22+1)*2</f>
+        <v>42</v>
+      </c>
+    </row>
+    <row r="29" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B29" t="s">
+        <v>78</v>
+      </c>
+      <c r="C29" s="13">
+        <f>(C24*C25*C26)+ (N28*N29*N30) + (N37*N38*N39) + (N46*N47*N48) + (N55*N56*N57)</f>
+        <v>1566292</v>
+      </c>
       <c r="J29" s="12"/>
-    </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="M29" t="s">
+        <v>36</v>
+      </c>
+      <c r="N29" s="12">
+        <f>(N25-N24+1)*2</f>
+        <v>17</v>
+      </c>
+    </row>
+    <row r="30" spans="1:14" x14ac:dyDescent="0.25">
       <c r="H30" s="12"/>
       <c r="J30" s="12"/>
-    </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="M30" s="12" t="s">
+        <v>48</v>
+      </c>
+      <c r="N30" s="12">
+        <f>(N27-N26+1)*2</f>
+        <v>32</v>
+      </c>
+    </row>
+    <row r="31" spans="1:14" x14ac:dyDescent="0.25">
       <c r="H31" s="12"/>
       <c r="J31" s="12"/>
-    </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="M31" t="s">
+        <v>43</v>
+      </c>
+      <c r="N31" s="16">
+        <f>(B20/4)*2</f>
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="32" spans="1:14" x14ac:dyDescent="0.25">
       <c r="J32" s="12"/>
-    </row>
-    <row r="33" spans="8:10" x14ac:dyDescent="0.25">
+      <c r="M32" t="s">
+        <v>39</v>
+      </c>
+      <c r="N32" s="16">
+        <f>N31+(3.25*B20*2)</f>
+        <v>35</v>
+      </c>
+    </row>
+    <row r="33" spans="8:14" x14ac:dyDescent="0.25">
       <c r="H33" s="12"/>
       <c r="J33" s="12"/>
-    </row>
-    <row r="34" spans="8:10" x14ac:dyDescent="0.25">
+      <c r="M33" s="12" t="s">
+        <v>44</v>
+      </c>
+      <c r="N33" s="16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="8:14" x14ac:dyDescent="0.25">
       <c r="H34" s="12"/>
+      <c r="M34" s="12" t="s">
+        <v>45</v>
+      </c>
+      <c r="N34" s="16">
+        <f>N33+(1.25*B20*2)</f>
+        <v>12.5</v>
+      </c>
+    </row>
+    <row r="35" spans="8:14" x14ac:dyDescent="0.25">
+      <c r="M35" s="12" t="s">
+        <v>53</v>
+      </c>
+      <c r="N35" s="16">
+        <f>(B20/4)*2</f>
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="36" spans="8:14" x14ac:dyDescent="0.25">
+      <c r="M36" s="12" t="s">
+        <v>54</v>
+      </c>
+      <c r="N36" s="16">
+        <f>N35+(2.5*B20*2)</f>
+        <v>27.5</v>
+      </c>
+    </row>
+    <row r="37" spans="8:14" x14ac:dyDescent="0.25">
+      <c r="M37" t="s">
+        <v>46</v>
+      </c>
+      <c r="N37" s="12">
+        <f>(N32-N31+1)*2</f>
+        <v>67</v>
+      </c>
+    </row>
+    <row r="38" spans="8:14" x14ac:dyDescent="0.25">
+      <c r="M38" t="s">
+        <v>47</v>
+      </c>
+      <c r="N38" s="12">
+        <f>(N34-N33+1)*2</f>
+        <v>27</v>
+      </c>
+    </row>
+    <row r="39" spans="8:14" x14ac:dyDescent="0.25">
+      <c r="M39" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="N39" s="12">
+        <f>(N36-N35+1)*2</f>
+        <v>52</v>
+      </c>
+    </row>
+    <row r="40" spans="8:14" x14ac:dyDescent="0.25">
+      <c r="M40" t="s">
+        <v>59</v>
+      </c>
+      <c r="N40" s="16">
+        <f>(B20/4)*4</f>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="41" spans="8:14" x14ac:dyDescent="0.25">
+      <c r="M41" t="s">
+        <v>60</v>
+      </c>
+      <c r="N41" s="16">
+        <f>N40+(2.5*B20*4)</f>
+        <v>55</v>
+      </c>
+    </row>
+    <row r="42" spans="8:14" x14ac:dyDescent="0.25">
+      <c r="M42" s="12" t="s">
+        <v>61</v>
+      </c>
+      <c r="N42" s="16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="8:14" x14ac:dyDescent="0.25">
+      <c r="M43" s="12" t="s">
+        <v>62</v>
+      </c>
+      <c r="N43" s="16">
+        <f>B20*4</f>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="44" spans="8:14" x14ac:dyDescent="0.25">
+      <c r="M44" s="12" t="s">
+        <v>63</v>
+      </c>
+      <c r="N44" s="16">
+        <f>(B20/4)*4</f>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="45" spans="8:14" x14ac:dyDescent="0.25">
+      <c r="M45" s="12" t="s">
+        <v>64</v>
+      </c>
+      <c r="N45" s="16">
+        <f>N44+(2*B20*4)</f>
+        <v>45</v>
+      </c>
+    </row>
+    <row r="46" spans="8:14" x14ac:dyDescent="0.25">
+      <c r="M46" t="s">
+        <v>65</v>
+      </c>
+      <c r="N46" s="12">
+        <f>(N41-N40+1)*2</f>
+        <v>102</v>
+      </c>
+    </row>
+    <row r="47" spans="8:14" x14ac:dyDescent="0.25">
+      <c r="M47" t="s">
+        <v>66</v>
+      </c>
+      <c r="N47" s="12">
+        <f>(N43-N42+1)*2</f>
+        <v>42</v>
+      </c>
+    </row>
+    <row r="48" spans="8:14" x14ac:dyDescent="0.25">
+      <c r="M48" s="12" t="s">
+        <v>67</v>
+      </c>
+      <c r="N48" s="12">
+        <f>(N45-N44+1)*2</f>
+        <v>82</v>
+      </c>
+    </row>
+    <row r="49" spans="13:14" x14ac:dyDescent="0.25">
+      <c r="M49" t="s">
+        <v>68</v>
+      </c>
+      <c r="N49" s="16">
+        <f>(B20/4)*8</f>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="50" spans="13:14" x14ac:dyDescent="0.25">
+      <c r="M50" t="s">
+        <v>69</v>
+      </c>
+      <c r="N50" s="16">
+        <f>N49+(1.75*B20*8)</f>
+        <v>80</v>
+      </c>
+    </row>
+    <row r="51" spans="13:14" x14ac:dyDescent="0.25">
+      <c r="M51" s="12" t="s">
+        <v>70</v>
+      </c>
+      <c r="N51" s="16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="13:14" x14ac:dyDescent="0.25">
+      <c r="M52" s="12" t="s">
+        <v>71</v>
+      </c>
+      <c r="N52" s="16">
+        <f>0.75*B20*8</f>
+        <v>30</v>
+      </c>
+    </row>
+    <row r="53" spans="13:14" x14ac:dyDescent="0.25">
+      <c r="M53" s="12" t="s">
+        <v>72</v>
+      </c>
+      <c r="N53" s="16">
+        <f>(B20/4)*8</f>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="54" spans="13:14" x14ac:dyDescent="0.25">
+      <c r="M54" s="12" t="s">
+        <v>73</v>
+      </c>
+      <c r="N54" s="16">
+        <f>N53+(1.5*B20*8)</f>
+        <v>70</v>
+      </c>
+    </row>
+    <row r="55" spans="13:14" x14ac:dyDescent="0.25">
+      <c r="M55" t="s">
+        <v>74</v>
+      </c>
+      <c r="N55" s="12">
+        <f>(N50-N49+1)*2</f>
+        <v>142</v>
+      </c>
+    </row>
+    <row r="56" spans="13:14" x14ac:dyDescent="0.25">
+      <c r="M56" t="s">
+        <v>76</v>
+      </c>
+      <c r="N56" s="12">
+        <f>(N52-N51+1)*2</f>
+        <v>62</v>
+      </c>
+    </row>
+    <row r="57" spans="13:14" x14ac:dyDescent="0.25">
+      <c r="M57" s="12" t="s">
+        <v>75</v>
+      </c>
+      <c r="N57" s="12">
+        <f>(N54-N53+1)*2</f>
+        <v>122</v>
+      </c>
+    </row>
+    <row r="58" spans="13:14" x14ac:dyDescent="0.25">
+      <c r="M58" t="s">
+        <v>26</v>
+      </c>
+      <c r="N58" s="16">
+        <f>(B20/4)*16</f>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="59" spans="13:14" x14ac:dyDescent="0.25">
+      <c r="M59" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="N59" s="16">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="60" spans="13:14" x14ac:dyDescent="0.25">
+      <c r="M60" t="s">
+        <v>56</v>
+      </c>
+      <c r="N60" s="16">
+        <f>N57/2</f>
+        <v>61</v>
+      </c>
+    </row>
+    <row r="61" spans="13:14" x14ac:dyDescent="0.25">
+      <c r="M61" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="N61" s="16">
+        <f>B20*16</f>
+        <v>80</v>
+      </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="A2:N16">
@@ -5454,10 +6197,10 @@
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet6"/>
-  <dimension ref="A1:N21"/>
+  <dimension ref="A1:N48"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="J21" sqref="J21"/>
+    <sheetView topLeftCell="A7" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="E24" sqref="E24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -5540,31 +6283,31 @@
       </c>
       <c r="F2" s="5">
         <f>($C$11/A2)+2</f>
-        <v>202</v>
+        <v>42</v>
       </c>
       <c r="G2" s="5">
         <f>($C$12/B2)+2</f>
-        <v>82</v>
+        <v>22</v>
       </c>
       <c r="H2" s="5">
         <f>($C$13/C2)+2</f>
-        <v>82</v>
+        <v>32</v>
       </c>
       <c r="I2" s="5">
         <f t="shared" ref="I2" si="1">F2*G2*H2</f>
-        <v>1358248</v>
+        <v>29568</v>
       </c>
       <c r="J2" s="5">
         <f t="shared" ref="J2" si="2">4*F2*G2+4*G2*H2+4*F2*H2</f>
-        <v>159408</v>
+        <v>11888</v>
       </c>
       <c r="K2" s="5">
         <f t="shared" ref="K2" si="3">J2*E2</f>
-        <v>1275264</v>
+        <v>95104</v>
       </c>
       <c r="L2" s="5">
         <f>K2/$C$14*100</f>
-        <v>12.453749999999999</v>
+        <v>49.533333333333331</v>
       </c>
       <c r="M2" s="6" t="b">
         <f>IF((F2-FLOOR(F2,1))=0,IF((G2-FLOOR(G2,1))=0,IF((H2-FLOOR(H2,1))=0,TRUE,FALSE),FALSE),FALSE)</f>
@@ -5595,31 +6338,31 @@
       </c>
       <c r="F3" s="5">
         <f>($C$11/A3)+2</f>
-        <v>102</v>
+        <v>22</v>
       </c>
       <c r="G3" s="5">
         <f>($C$12/B3)+2</f>
-        <v>82</v>
+        <v>22</v>
       </c>
       <c r="H3" s="5">
         <f>($C$13/C3)+2</f>
-        <v>82</v>
+        <v>32</v>
       </c>
       <c r="I3" s="5">
         <f t="shared" ref="I3" si="5">F3*G3*H3</f>
-        <v>685848</v>
+        <v>15488</v>
       </c>
       <c r="J3" s="5">
         <f t="shared" ref="J3" si="6">4*F3*G3+4*G3*H3+4*F3*H3</f>
-        <v>93808</v>
+        <v>7568</v>
       </c>
       <c r="K3" s="5">
         <f t="shared" ref="K3" si="7">J3*E3</f>
-        <v>1500928</v>
+        <v>121088</v>
       </c>
       <c r="L3" s="5">
         <f>K3/$C$14*100</f>
-        <v>14.657500000000001</v>
+        <v>63.06666666666667</v>
       </c>
       <c r="M3" s="6" t="b">
         <f>IF((F3-FLOOR(F3,1))=0,IF((G3-FLOOR(G3,1))=0,IF((H3-FLOOR(H3,1))=0,TRUE,FALSE),FALSE),FALSE)</f>
@@ -5646,10 +6389,27 @@
         <v>10</v>
       </c>
       <c r="B7">
-        <v>40</v>
+        <v>10</v>
       </c>
       <c r="D7" s="10" t="s">
         <v>18</v>
+      </c>
+      <c r="M7" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="M8" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="M9" t="s">
+        <v>38</v>
+      </c>
+      <c r="N9" s="16">
+        <f>0.25*(B11-4)*B7</f>
+        <v>10</v>
       </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.25">
@@ -5660,21 +6420,34 @@
       <c r="C10" s="1" t="s">
         <v>12</v>
       </c>
+      <c r="M10" t="s">
+        <v>41</v>
+      </c>
+      <c r="N10" s="16">
+        <f>N9+(4*B7)</f>
+        <v>50</v>
+      </c>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>4</v>
       </c>
       <c r="B11" s="1">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C11" s="3">
         <f>$B$7*B11</f>
-        <v>400</v>
+        <v>80</v>
       </c>
       <c r="E11" s="12"/>
       <c r="H11" s="12"/>
       <c r="J11" s="12"/>
+      <c r="M11" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="N11" s="16">
+        <v>0</v>
+      </c>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
@@ -5685,24 +6458,38 @@
       </c>
       <c r="C12" s="3">
         <f t="shared" ref="C12:C13" si="8">$B$7*B12</f>
-        <v>160</v>
+        <v>40</v>
       </c>
       <c r="E12" s="12"/>
       <c r="H12" s="12"/>
       <c r="J12" s="12"/>
+      <c r="M12" s="12" t="s">
+        <v>42</v>
+      </c>
+      <c r="N12" s="16">
+        <f>1.5*B7</f>
+        <v>15</v>
+      </c>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>6</v>
       </c>
       <c r="B13" s="1">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C13" s="3">
         <f t="shared" si="8"/>
-        <v>160</v>
+        <v>60</v>
       </c>
       <c r="J13" s="12"/>
+      <c r="M13" s="12" t="s">
+        <v>51</v>
+      </c>
+      <c r="N13" s="16">
+        <f>(B13/2-1.5)*B7</f>
+        <v>15</v>
+      </c>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B14" s="1" t="s">
@@ -5710,35 +6497,337 @@
       </c>
       <c r="C14" s="3">
         <f>C11*C12*C13</f>
-        <v>10240000</v>
+        <v>192000</v>
       </c>
       <c r="H14" s="12"/>
       <c r="J14" s="12"/>
+      <c r="M14" s="12" t="s">
+        <v>52</v>
+      </c>
+      <c r="N14" s="16">
+        <f>N13+(3*B7)</f>
+        <v>45</v>
+      </c>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="H15" s="12"/>
       <c r="J15" s="12"/>
+      <c r="M15" t="s">
+        <v>35</v>
+      </c>
+      <c r="N15" s="12">
+        <f>(N10-N9+1)*2</f>
+        <v>82</v>
+      </c>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B16" t="s">
+        <v>78</v>
+      </c>
+      <c r="C16" s="13">
+        <f>(C11*C12*C13)+ (N15*N16*N17) + (N24*N25*N26) + (N33*N34*N35) + (N42*N43*N44)</f>
+        <v>12063952</v>
+      </c>
       <c r="J16" s="12"/>
-    </row>
-    <row r="17" spans="8:10" x14ac:dyDescent="0.25">
+      <c r="M16" t="s">
+        <v>36</v>
+      </c>
+      <c r="N16" s="12">
+        <f>(N12-N11+1)*2</f>
+        <v>32</v>
+      </c>
+    </row>
+    <row r="17" spans="8:14" x14ac:dyDescent="0.25">
       <c r="H17" s="12"/>
       <c r="J17" s="12"/>
-    </row>
-    <row r="18" spans="8:10" x14ac:dyDescent="0.25">
+      <c r="M17" s="12" t="s">
+        <v>48</v>
+      </c>
+      <c r="N17" s="12">
+        <f>(N14-N13+1)*2</f>
+        <v>62</v>
+      </c>
+    </row>
+    <row r="18" spans="8:14" x14ac:dyDescent="0.25">
       <c r="H18" s="12"/>
       <c r="J18" s="12"/>
-    </row>
-    <row r="19" spans="8:10" x14ac:dyDescent="0.25">
+      <c r="M18" t="s">
+        <v>43</v>
+      </c>
+      <c r="N18" s="16">
+        <f>(B7/4)*2</f>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="19" spans="8:14" x14ac:dyDescent="0.25">
       <c r="J19" s="12"/>
-    </row>
-    <row r="20" spans="8:10" x14ac:dyDescent="0.25">
+      <c r="M19" t="s">
+        <v>39</v>
+      </c>
+      <c r="N19" s="16">
+        <f>N18+(3.25*B7*2)</f>
+        <v>70</v>
+      </c>
+    </row>
+    <row r="20" spans="8:14" x14ac:dyDescent="0.25">
       <c r="H20" s="12"/>
       <c r="J20" s="12"/>
-    </row>
-    <row r="21" spans="8:10" x14ac:dyDescent="0.25">
+      <c r="M20" s="12" t="s">
+        <v>44</v>
+      </c>
+      <c r="N20" s="16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="8:14" x14ac:dyDescent="0.25">
       <c r="H21" s="12"/>
+      <c r="M21" s="12" t="s">
+        <v>45</v>
+      </c>
+      <c r="N21" s="16">
+        <f>N20+(1.25*B7*2)</f>
+        <v>25</v>
+      </c>
+    </row>
+    <row r="22" spans="8:14" x14ac:dyDescent="0.25">
+      <c r="M22" s="12" t="s">
+        <v>53</v>
+      </c>
+      <c r="N22" s="16">
+        <f>(B7/4)*2</f>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="23" spans="8:14" x14ac:dyDescent="0.25">
+      <c r="M23" s="12" t="s">
+        <v>54</v>
+      </c>
+      <c r="N23" s="16">
+        <f>N22+(2.5*B7*2)</f>
+        <v>55</v>
+      </c>
+    </row>
+    <row r="24" spans="8:14" x14ac:dyDescent="0.25">
+      <c r="M24" t="s">
+        <v>46</v>
+      </c>
+      <c r="N24" s="12">
+        <f>(N19-N18+1)*2</f>
+        <v>132</v>
+      </c>
+    </row>
+    <row r="25" spans="8:14" x14ac:dyDescent="0.25">
+      <c r="M25" t="s">
+        <v>47</v>
+      </c>
+      <c r="N25" s="12">
+        <f>(N21-N20+1)*2</f>
+        <v>52</v>
+      </c>
+    </row>
+    <row r="26" spans="8:14" x14ac:dyDescent="0.25">
+      <c r="M26" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="N26" s="12">
+        <f>(N23-N22+1)*2</f>
+        <v>102</v>
+      </c>
+    </row>
+    <row r="27" spans="8:14" x14ac:dyDescent="0.25">
+      <c r="M27" t="s">
+        <v>59</v>
+      </c>
+      <c r="N27" s="16">
+        <f>(B7/4)*4</f>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="28" spans="8:14" x14ac:dyDescent="0.25">
+      <c r="M28" t="s">
+        <v>60</v>
+      </c>
+      <c r="N28" s="16">
+        <f>N27+(2.5*B7*4)</f>
+        <v>110</v>
+      </c>
+    </row>
+    <row r="29" spans="8:14" x14ac:dyDescent="0.25">
+      <c r="M29" s="12" t="s">
+        <v>61</v>
+      </c>
+      <c r="N29" s="16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="8:14" x14ac:dyDescent="0.25">
+      <c r="M30" s="12" t="s">
+        <v>62</v>
+      </c>
+      <c r="N30" s="16">
+        <f>B7*4</f>
+        <v>40</v>
+      </c>
+    </row>
+    <row r="31" spans="8:14" x14ac:dyDescent="0.25">
+      <c r="M31" s="12" t="s">
+        <v>63</v>
+      </c>
+      <c r="N31" s="16">
+        <f>(B7/4)*4</f>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="32" spans="8:14" x14ac:dyDescent="0.25">
+      <c r="M32" s="12" t="s">
+        <v>64</v>
+      </c>
+      <c r="N32" s="16">
+        <f>N31+(2*B7*4)</f>
+        <v>90</v>
+      </c>
+    </row>
+    <row r="33" spans="13:14" x14ac:dyDescent="0.25">
+      <c r="M33" t="s">
+        <v>65</v>
+      </c>
+      <c r="N33" s="12">
+        <f>(N28-N27+1)*2</f>
+        <v>202</v>
+      </c>
+    </row>
+    <row r="34" spans="13:14" x14ac:dyDescent="0.25">
+      <c r="M34" t="s">
+        <v>66</v>
+      </c>
+      <c r="N34" s="12">
+        <f>(N30-N29+1)*2</f>
+        <v>82</v>
+      </c>
+    </row>
+    <row r="35" spans="13:14" x14ac:dyDescent="0.25">
+      <c r="M35" s="12" t="s">
+        <v>67</v>
+      </c>
+      <c r="N35" s="12">
+        <f>(N32-N31+1)*2</f>
+        <v>162</v>
+      </c>
+    </row>
+    <row r="36" spans="13:14" x14ac:dyDescent="0.25">
+      <c r="M36" t="s">
+        <v>68</v>
+      </c>
+      <c r="N36" s="16">
+        <f>(B7/4)*8</f>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="37" spans="13:14" x14ac:dyDescent="0.25">
+      <c r="M37" t="s">
+        <v>69</v>
+      </c>
+      <c r="N37" s="16">
+        <f>N36+(1.75*B7*8)</f>
+        <v>160</v>
+      </c>
+    </row>
+    <row r="38" spans="13:14" x14ac:dyDescent="0.25">
+      <c r="M38" s="12" t="s">
+        <v>70</v>
+      </c>
+      <c r="N38" s="16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="13:14" x14ac:dyDescent="0.25">
+      <c r="M39" s="12" t="s">
+        <v>71</v>
+      </c>
+      <c r="N39" s="16">
+        <f>0.75*B7*8</f>
+        <v>60</v>
+      </c>
+    </row>
+    <row r="40" spans="13:14" x14ac:dyDescent="0.25">
+      <c r="M40" s="12" t="s">
+        <v>72</v>
+      </c>
+      <c r="N40" s="16">
+        <f>(B7/4)*8</f>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="41" spans="13:14" x14ac:dyDescent="0.25">
+      <c r="M41" s="12" t="s">
+        <v>73</v>
+      </c>
+      <c r="N41" s="16">
+        <f>N40+(1.5*B7*8)</f>
+        <v>140</v>
+      </c>
+    </row>
+    <row r="42" spans="13:14" x14ac:dyDescent="0.25">
+      <c r="M42" t="s">
+        <v>74</v>
+      </c>
+      <c r="N42" s="12">
+        <f>(N37-N36+1)*2</f>
+        <v>282</v>
+      </c>
+    </row>
+    <row r="43" spans="13:14" x14ac:dyDescent="0.25">
+      <c r="M43" t="s">
+        <v>76</v>
+      </c>
+      <c r="N43" s="12">
+        <f>(N39-N38+1)*2</f>
+        <v>122</v>
+      </c>
+    </row>
+    <row r="44" spans="13:14" x14ac:dyDescent="0.25">
+      <c r="M44" s="12" t="s">
+        <v>75</v>
+      </c>
+      <c r="N44" s="12">
+        <f>(N41-N40+1)*2</f>
+        <v>242</v>
+      </c>
+    </row>
+    <row r="45" spans="13:14" x14ac:dyDescent="0.25">
+      <c r="M45" t="s">
+        <v>26</v>
+      </c>
+      <c r="N45" s="16">
+        <f>(B7/4)*16</f>
+        <v>40</v>
+      </c>
+    </row>
+    <row r="46" spans="13:14" x14ac:dyDescent="0.25">
+      <c r="M46" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="N46" s="16">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="47" spans="13:14" x14ac:dyDescent="0.25">
+      <c r="M47" t="s">
+        <v>56</v>
+      </c>
+      <c r="N47" s="16">
+        <f>N44/2</f>
+        <v>121</v>
+      </c>
+    </row>
+    <row r="48" spans="13:14" x14ac:dyDescent="0.25">
+      <c r="M48" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="N48" s="16">
+        <f>B7*16</f>
+        <v>160</v>
+      </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="A2:N2">

</xml_diff>

<commit_message>
Release 1.0.2 -- see release notes in /version
</commit_message>
<xml_diff>
--- a/LUMA/tools/SizingGuide.xlsx
+++ b/LUMA/tools/SizingGuide.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9372" tabRatio="573" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9372" tabRatio="573"/>
   </bookViews>
   <sheets>
     <sheet name="Archer" sheetId="11" r:id="rId1"/>
@@ -813,8 +813,8 @@
   <sheetPr codeName="Sheet4"/>
   <dimension ref="A1:N61"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B29" sqref="B29:C29"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -880,49 +880,49 @@
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="4">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B2" s="4">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="C2" s="4">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="D2" s="5">
         <f t="shared" ref="D2:D16" si="0">E2/$B$19</f>
-        <v>0.33333333333333331</v>
+        <v>4</v>
       </c>
       <c r="E2" s="5">
         <f t="shared" ref="E2:E16" si="1">A2*B2*C2</f>
-        <v>8</v>
+        <v>96</v>
       </c>
       <c r="F2" s="5">
         <f t="shared" ref="F2:F16" si="2">($C$24/A2)+2</f>
-        <v>98</v>
+        <v>22</v>
       </c>
       <c r="G2" s="5">
         <f t="shared" ref="G2:G16" si="3">($C$25/B2)+2</f>
-        <v>50</v>
+        <v>12</v>
       </c>
       <c r="H2" s="5">
         <f t="shared" ref="H2:H16" si="4">($C$26/C2)+2</f>
-        <v>74</v>
+        <v>12</v>
       </c>
       <c r="I2" s="5">
         <f t="shared" ref="I2:I16" si="5">F2*G2*H2</f>
-        <v>362600</v>
+        <v>3168</v>
       </c>
       <c r="J2" s="5">
         <f t="shared" ref="J2:J16" si="6">4*F2*G2+4*G2*H2+4*F2*H2</f>
-        <v>63408</v>
+        <v>2688</v>
       </c>
       <c r="K2" s="5">
         <f t="shared" ref="K2:K16" si="7">J2*E2</f>
-        <v>507264</v>
+        <v>258048</v>
       </c>
       <c r="L2" s="5">
         <f t="shared" ref="L2:L16" si="8">K2/$C$27*100</f>
-        <v>19.111689814814813</v>
+        <v>134.4</v>
       </c>
       <c r="M2" s="6" t="b">
         <f>IF((F2-FLOOR(F2,1))=0,IF((G2-FLOOR(G2,1))=0,IF((H2-FLOOR(H2,1))=0,TRUE,FALSE),FALSE),FALSE)</f>
@@ -930,54 +930,54 @@
       </c>
       <c r="N2" s="6" t="b">
         <f>IF(($D2-FLOOR($D2,1))=0,TRUE,FALSE)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" s="4">
-        <v>16</v>
+        <v>4</v>
       </c>
       <c r="B3" s="4">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="C3" s="4">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="D3" s="5">
         <f t="shared" si="0"/>
-        <v>32</v>
+        <v>2</v>
       </c>
       <c r="E3" s="5">
         <f t="shared" si="1"/>
-        <v>768</v>
+        <v>48</v>
       </c>
       <c r="F3" s="5">
         <f t="shared" si="2"/>
-        <v>14</v>
+        <v>22</v>
       </c>
       <c r="G3" s="5">
         <f t="shared" si="3"/>
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="H3" s="5">
         <f t="shared" si="4"/>
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="I3" s="5">
         <f t="shared" si="5"/>
-        <v>5096</v>
+        <v>5808</v>
       </c>
       <c r="J3" s="5">
         <f t="shared" si="6"/>
-        <v>3696</v>
+        <v>4048</v>
       </c>
       <c r="K3" s="5">
         <f t="shared" si="7"/>
-        <v>2838528</v>
+        <v>194304</v>
       </c>
       <c r="L3" s="5">
         <f t="shared" si="8"/>
-        <v>106.94444444444444</v>
+        <v>101.2</v>
       </c>
       <c r="M3" s="6" t="b">
         <f>IF((F3-FLOOR(F3,1))=0,IF((G3-FLOOR(G3,1))=0,IF((H3-FLOOR(H3,1))=0,TRUE,FALSE),FALSE),FALSE)</f>
@@ -990,53 +990,53 @@
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" s="4">
-        <v>20</v>
+        <v>4</v>
       </c>
       <c r="B4" s="4">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="C4" s="4">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="D4" s="5">
         <f t="shared" si="0"/>
-        <v>25</v>
+        <v>1</v>
       </c>
       <c r="E4" s="5">
         <f t="shared" si="1"/>
-        <v>600</v>
+        <v>24</v>
       </c>
       <c r="F4" s="5">
         <f t="shared" si="2"/>
-        <v>11.6</v>
+        <v>22</v>
       </c>
       <c r="G4" s="5">
         <f t="shared" si="3"/>
-        <v>21.2</v>
+        <v>22</v>
       </c>
       <c r="H4" s="5">
         <f t="shared" si="4"/>
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="I4" s="5">
         <f t="shared" si="5"/>
-        <v>6393.92</v>
+        <v>10648</v>
       </c>
       <c r="J4" s="5">
         <f t="shared" si="6"/>
-        <v>4394.8799999999992</v>
+        <v>5808</v>
       </c>
       <c r="K4" s="5">
         <f t="shared" si="7"/>
-        <v>2636927.9999999995</v>
+        <v>139392</v>
       </c>
       <c r="L4" s="5">
         <f t="shared" si="8"/>
-        <v>99.348958333333314</v>
+        <v>72.599999999999994</v>
       </c>
       <c r="M4" s="6" t="b">
         <f t="shared" ref="M4:M6" si="10">IF((F4-FLOOR(F4,1))=0,IF((G4-FLOOR(G4,1))=0,IF((H4-FLOOR(H4,1))=0,TRUE,FALSE),FALSE),FALSE)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N4" s="6" t="b">
         <f t="shared" si="9"/>
@@ -1045,53 +1045,53 @@
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" s="4">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="B5" s="4">
         <v>10</v>
       </c>
       <c r="C5" s="4">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="D5" s="5">
         <f t="shared" si="0"/>
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="E5" s="5">
         <f t="shared" si="1"/>
-        <v>120</v>
+        <v>480</v>
       </c>
       <c r="F5" s="5">
         <f t="shared" si="2"/>
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="G5" s="5">
         <f t="shared" si="3"/>
-        <v>11.6</v>
+        <v>6</v>
       </c>
       <c r="H5" s="5">
         <f t="shared" si="4"/>
-        <v>146</v>
+        <v>12</v>
       </c>
       <c r="I5" s="5">
         <f t="shared" si="5"/>
-        <v>30484.799999999999</v>
+        <v>864</v>
       </c>
       <c r="J5" s="5">
         <f t="shared" si="6"/>
-        <v>18121.599999999999</v>
+        <v>1152</v>
       </c>
       <c r="K5" s="5">
         <f t="shared" si="7"/>
-        <v>2174592</v>
+        <v>552960</v>
       </c>
       <c r="L5" s="5">
         <f t="shared" si="8"/>
-        <v>81.929976851851848</v>
+        <v>288</v>
       </c>
       <c r="M5" s="6" t="b">
         <f t="shared" si="10"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N5" s="6" t="b">
         <f t="shared" si="9"/>
@@ -1100,53 +1100,53 @@
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" s="4">
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="B6" s="4">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C6" s="4">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="D6" s="5">
         <f t="shared" si="0"/>
-        <v>20</v>
+        <v>50</v>
       </c>
       <c r="E6" s="5">
         <f t="shared" si="1"/>
-        <v>480</v>
+        <v>1200</v>
       </c>
       <c r="F6" s="5">
         <f t="shared" si="2"/>
-        <v>18</v>
+        <v>6</v>
       </c>
       <c r="G6" s="5">
         <f t="shared" si="3"/>
-        <v>21.2</v>
+        <v>12</v>
       </c>
       <c r="H6" s="5">
         <f t="shared" si="4"/>
-        <v>20</v>
+        <v>6</v>
       </c>
       <c r="I6" s="5">
         <f t="shared" si="5"/>
-        <v>7631.9999999999991</v>
+        <v>432</v>
       </c>
       <c r="J6" s="5">
         <f t="shared" si="6"/>
-        <v>4662.3999999999996</v>
+        <v>720</v>
       </c>
       <c r="K6" s="5">
         <f t="shared" si="7"/>
-        <v>2237952</v>
+        <v>864000</v>
       </c>
       <c r="L6" s="5">
         <f t="shared" si="8"/>
-        <v>84.317129629629633</v>
+        <v>450</v>
       </c>
       <c r="M6" s="6" t="b">
         <f t="shared" si="10"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N6" s="6" t="b">
         <f t="shared" si="9"/>
@@ -1173,31 +1173,31 @@
       </c>
       <c r="F7" s="5">
         <f t="shared" si="2"/>
-        <v>18</v>
+        <v>8.6666666666666679</v>
       </c>
       <c r="G7" s="5">
         <f t="shared" si="3"/>
-        <v>10</v>
+        <v>5.3333333333333339</v>
       </c>
       <c r="H7" s="5">
         <f t="shared" si="4"/>
-        <v>16.399999999999999</v>
+        <v>8</v>
       </c>
       <c r="I7" s="5">
         <f t="shared" si="5"/>
-        <v>2951.9999999999995</v>
+        <v>369.77777777777789</v>
       </c>
       <c r="J7" s="5">
         <f t="shared" si="6"/>
-        <v>2556.8000000000002</v>
+        <v>632.88888888888903</v>
       </c>
       <c r="K7" s="5">
         <f t="shared" si="7"/>
-        <v>3681792.0000000005</v>
+        <v>911360.00000000023</v>
       </c>
       <c r="L7" s="5">
         <f t="shared" si="8"/>
-        <v>138.7152777777778</v>
+        <v>474.6666666666668</v>
       </c>
       <c r="M7" s="6" t="b">
         <f>IF((F7-FLOOR(F7,1))=0,IF((G7-FLOOR(G7,1))=0,IF((H7-FLOOR(H7,1))=0,TRUE,FALSE),FALSE),FALSE)</f>
@@ -1228,31 +1228,31 @@
       </c>
       <c r="F8" s="5">
         <f t="shared" si="2"/>
-        <v>18</v>
+        <v>8.6666666666666679</v>
       </c>
       <c r="G8" s="5">
         <f t="shared" si="3"/>
-        <v>11.6</v>
+        <v>6</v>
       </c>
       <c r="H8" s="5">
         <f t="shared" si="4"/>
-        <v>74</v>
+        <v>32</v>
       </c>
       <c r="I8" s="5">
         <f t="shared" si="5"/>
-        <v>15451.199999999999</v>
+        <v>1664.0000000000002</v>
       </c>
       <c r="J8" s="5">
         <f t="shared" si="6"/>
-        <v>9596.7999999999993</v>
+        <v>2085.3333333333335</v>
       </c>
       <c r="K8" s="5">
         <f t="shared" si="7"/>
-        <v>2303232</v>
+        <v>500480.00000000006</v>
       </c>
       <c r="L8" s="5">
         <f t="shared" si="8"/>
-        <v>86.776620370370367</v>
+        <v>260.66666666666669</v>
       </c>
       <c r="M8" s="6" t="b">
         <f t="shared" ref="M8:M16" si="11">IF((F8-FLOOR(F8,1))=0,IF((G8-FLOOR(G8,1))=0,IF((H8-FLOOR(H8,1))=0,TRUE,FALSE),FALSE),FALSE)</f>
@@ -1283,35 +1283,35 @@
       </c>
       <c r="F9" s="5">
         <f t="shared" si="2"/>
-        <v>26</v>
+        <v>12</v>
       </c>
       <c r="G9" s="5">
         <f t="shared" si="3"/>
-        <v>21.2</v>
+        <v>10</v>
       </c>
       <c r="H9" s="5">
         <f t="shared" si="4"/>
-        <v>38</v>
+        <v>17</v>
       </c>
       <c r="I9" s="5">
         <f t="shared" si="5"/>
-        <v>20945.599999999999</v>
+        <v>2040</v>
       </c>
       <c r="J9" s="5">
         <f t="shared" si="6"/>
-        <v>9379.2000000000007</v>
+        <v>1976</v>
       </c>
       <c r="K9" s="5">
         <f t="shared" si="7"/>
-        <v>1500672</v>
+        <v>316160</v>
       </c>
       <c r="L9" s="5">
         <f t="shared" si="8"/>
-        <v>56.539351851851848</v>
+        <v>164.66666666666669</v>
       </c>
       <c r="M9" s="6" t="b">
         <f t="shared" si="11"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N9" s="6" t="b">
         <f t="shared" si="9"/>
@@ -1338,35 +1338,35 @@
       </c>
       <c r="F10" s="5">
         <f t="shared" si="2"/>
-        <v>21.2</v>
+        <v>10</v>
       </c>
       <c r="G10" s="5">
         <f t="shared" si="3"/>
-        <v>26</v>
+        <v>12</v>
       </c>
       <c r="H10" s="5">
         <f t="shared" si="4"/>
-        <v>38</v>
+        <v>17</v>
       </c>
       <c r="I10" s="5">
         <f t="shared" si="5"/>
-        <v>20945.599999999999</v>
+        <v>2040</v>
       </c>
       <c r="J10" s="5">
         <f t="shared" si="6"/>
-        <v>9379.1999999999989</v>
+        <v>1976</v>
       </c>
       <c r="K10" s="5">
         <f t="shared" si="7"/>
-        <v>1500671.9999999998</v>
+        <v>316160</v>
       </c>
       <c r="L10" s="5">
         <f t="shared" si="8"/>
-        <v>56.539351851851841</v>
+        <v>164.66666666666669</v>
       </c>
       <c r="M10" s="6" t="b">
         <f t="shared" si="11"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N10" s="6" t="b">
         <f t="shared" si="9"/>
@@ -1393,35 +1393,35 @@
       </c>
       <c r="F11" s="5">
         <f t="shared" si="2"/>
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="G11" s="5">
         <f t="shared" si="3"/>
-        <v>21.2</v>
+        <v>10</v>
       </c>
       <c r="H11" s="5">
         <f t="shared" si="4"/>
-        <v>74</v>
+        <v>32</v>
       </c>
       <c r="I11" s="5">
         <f t="shared" si="5"/>
-        <v>21963.200000000001</v>
+        <v>2240</v>
       </c>
       <c r="J11" s="5">
         <f t="shared" si="6"/>
-        <v>11606.4</v>
+        <v>2456</v>
       </c>
       <c r="K11" s="5">
         <f t="shared" si="7"/>
-        <v>1857024</v>
+        <v>392960</v>
       </c>
       <c r="L11" s="5">
         <f t="shared" si="8"/>
-        <v>69.965277777777786</v>
+        <v>204.66666666666669</v>
       </c>
       <c r="M11" s="6" t="b">
         <f t="shared" si="11"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N11" s="6" t="b">
         <f t="shared" si="9"/>
@@ -1448,31 +1448,31 @@
       </c>
       <c r="F12" s="5">
         <f t="shared" si="2"/>
-        <v>26</v>
+        <v>12</v>
       </c>
       <c r="G12" s="5">
         <f t="shared" si="3"/>
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="H12" s="5">
         <f t="shared" si="4"/>
-        <v>26</v>
+        <v>12</v>
       </c>
       <c r="I12" s="5">
         <f t="shared" si="5"/>
-        <v>9464</v>
+        <v>1008</v>
       </c>
       <c r="J12" s="5">
         <f t="shared" si="6"/>
-        <v>5616</v>
+        <v>1248</v>
       </c>
       <c r="K12" s="5">
         <f t="shared" si="7"/>
-        <v>2156544</v>
+        <v>479232</v>
       </c>
       <c r="L12" s="5">
         <f t="shared" si="8"/>
-        <v>81.25</v>
+        <v>249.6</v>
       </c>
       <c r="M12" s="6" t="b">
         <f t="shared" si="11"/>
@@ -1503,31 +1503,31 @@
       </c>
       <c r="F13" s="5">
         <f t="shared" si="2"/>
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="G13" s="5">
         <f t="shared" si="3"/>
-        <v>26</v>
+        <v>12</v>
       </c>
       <c r="H13" s="5">
         <f t="shared" si="4"/>
-        <v>38</v>
+        <v>17</v>
       </c>
       <c r="I13" s="5">
         <f t="shared" si="5"/>
-        <v>13832</v>
+        <v>1428</v>
       </c>
       <c r="J13" s="5">
         <f t="shared" si="6"/>
-        <v>7536</v>
+        <v>1628</v>
       </c>
       <c r="K13" s="5">
         <f t="shared" si="7"/>
-        <v>1929216</v>
+        <v>416768</v>
       </c>
       <c r="L13" s="5">
         <f t="shared" si="8"/>
-        <v>72.68518518518519</v>
+        <v>217.06666666666666</v>
       </c>
       <c r="M13" s="6" t="b">
         <f t="shared" si="11"/>
@@ -1558,31 +1558,31 @@
       </c>
       <c r="F14" s="5">
         <f t="shared" si="2"/>
-        <v>26</v>
+        <v>12</v>
       </c>
       <c r="G14" s="5">
         <f t="shared" si="3"/>
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="H14" s="5">
         <f t="shared" si="4"/>
-        <v>38</v>
+        <v>17</v>
       </c>
       <c r="I14" s="5">
         <f t="shared" si="5"/>
-        <v>13832</v>
+        <v>1428</v>
       </c>
       <c r="J14" s="5">
         <f t="shared" si="6"/>
-        <v>7536</v>
+        <v>1628</v>
       </c>
       <c r="K14" s="5">
         <f t="shared" si="7"/>
-        <v>1929216</v>
+        <v>416768</v>
       </c>
       <c r="L14" s="5">
         <f t="shared" si="8"/>
-        <v>72.68518518518519</v>
+        <v>217.06666666666666</v>
       </c>
       <c r="M14" s="6" t="b">
         <f t="shared" si="11"/>
@@ -1613,35 +1613,35 @@
       </c>
       <c r="F15" s="5">
         <f t="shared" si="2"/>
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="G15" s="5">
         <f t="shared" si="3"/>
-        <v>11.6</v>
+        <v>6</v>
       </c>
       <c r="H15" s="5">
         <f t="shared" si="4"/>
-        <v>74</v>
+        <v>32</v>
       </c>
       <c r="I15" s="5">
         <f t="shared" si="5"/>
-        <v>12017.6</v>
+        <v>1344</v>
       </c>
       <c r="J15" s="5">
         <f t="shared" si="6"/>
-        <v>8227.2000000000007</v>
+        <v>1832</v>
       </c>
       <c r="K15" s="5">
         <f t="shared" si="7"/>
-        <v>2632704</v>
+        <v>586240</v>
       </c>
       <c r="L15" s="5">
         <f t="shared" si="8"/>
-        <v>99.18981481481481</v>
+        <v>305.33333333333331</v>
       </c>
       <c r="M15" s="6" t="b">
         <f t="shared" si="11"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N15" s="6" t="b">
         <f t="shared" si="9"/>
@@ -1668,35 +1668,35 @@
       </c>
       <c r="F16" s="5">
         <f t="shared" si="2"/>
-        <v>21.2</v>
+        <v>10</v>
       </c>
       <c r="G16" s="5">
         <f t="shared" si="3"/>
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="H16" s="5">
         <f t="shared" si="4"/>
-        <v>38</v>
+        <v>17</v>
       </c>
       <c r="I16" s="5">
         <f t="shared" si="5"/>
-        <v>11278.4</v>
+        <v>1190</v>
       </c>
       <c r="J16" s="5">
         <f t="shared" si="6"/>
-        <v>6537.6</v>
+        <v>1436</v>
       </c>
       <c r="K16" s="5">
         <f t="shared" si="7"/>
-        <v>2092032</v>
+        <v>459520</v>
       </c>
       <c r="L16" s="5">
         <f t="shared" si="8"/>
-        <v>78.819444444444443</v>
+        <v>239.33333333333334</v>
       </c>
       <c r="M16" s="6" t="b">
         <f t="shared" si="11"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N16" s="6" t="b">
         <f t="shared" si="9"/>
@@ -1719,7 +1719,7 @@
         <v>79</v>
       </c>
       <c r="B20" s="14">
-        <v>24</v>
+        <v>10</v>
       </c>
       <c r="D20" s="10" t="s">
         <v>18</v>
@@ -1736,7 +1736,7 @@
         <v>34</v>
       </c>
       <c r="B21" s="14">
-        <v>0</v>
+        <v>90</v>
       </c>
       <c r="F21" t="s">
         <v>25</v>
@@ -1757,28 +1757,28 @@
       </c>
       <c r="G22" s="13">
         <f>0.5*($C$24-$B$20*COS($B$21*PI()/180))</f>
-        <v>84</v>
+        <v>40</v>
       </c>
       <c r="H22" t="s">
         <v>29</v>
       </c>
       <c r="I22" s="13">
         <f>$C$24/4</f>
-        <v>48</v>
+        <v>20</v>
       </c>
       <c r="J22" t="s">
         <v>38</v>
       </c>
       <c r="K22" s="13">
         <f>$C$24/4</f>
-        <v>48</v>
+        <v>20</v>
       </c>
       <c r="M22" t="s">
         <v>38</v>
       </c>
       <c r="N22" s="16">
         <f>0.25*(B24-4)*B20</f>
-        <v>24</v>
+        <v>10</v>
       </c>
     </row>
     <row r="23" spans="1:14" x14ac:dyDescent="0.25">
@@ -1794,28 +1794,28 @@
       </c>
       <c r="G23" s="13">
         <f>0.5*($C$24-$B$20*SIN($B$21*PI()/180))</f>
-        <v>96</v>
+        <v>35</v>
       </c>
       <c r="H23" t="s">
         <v>30</v>
       </c>
       <c r="I23" s="13">
         <f>3*$C$24/4</f>
-        <v>144</v>
+        <v>60</v>
       </c>
       <c r="J23" t="s">
         <v>41</v>
       </c>
       <c r="K23" s="13">
         <f>3*$C$24/4</f>
-        <v>144</v>
+        <v>60</v>
       </c>
       <c r="M23" t="s">
         <v>41</v>
       </c>
       <c r="N23" s="16">
         <f>N22+(4*B20)</f>
-        <v>120</v>
+        <v>50</v>
       </c>
     </row>
     <row r="24" spans="1:14" x14ac:dyDescent="0.25">
@@ -1827,7 +1827,7 @@
       </c>
       <c r="C24" s="3">
         <f>$B$20*B24</f>
-        <v>192</v>
+        <v>80</v>
       </c>
       <c r="E24" s="12"/>
       <c r="F24" t="s">
@@ -1835,21 +1835,21 @@
       </c>
       <c r="G24" s="13">
         <f>C26/2</f>
-        <v>72</v>
+        <v>30</v>
       </c>
       <c r="H24" s="12" t="s">
         <v>31</v>
       </c>
       <c r="I24" s="13">
         <f>$C$25/4</f>
-        <v>24</v>
+        <v>10</v>
       </c>
       <c r="J24" s="12" t="s">
         <v>40</v>
       </c>
       <c r="K24" s="13">
         <f>$C$25/4</f>
-        <v>24</v>
+        <v>10</v>
       </c>
       <c r="M24" s="12" t="s">
         <v>40</v>
@@ -1867,7 +1867,7 @@
       </c>
       <c r="C25" s="3">
         <f t="shared" ref="C25" si="12">$B$20*B25</f>
-        <v>96</v>
+        <v>40</v>
       </c>
       <c r="E25" s="12"/>
       <c r="F25" t="s">
@@ -1875,28 +1875,28 @@
       </c>
       <c r="G25" s="12">
         <f>B20*COS(B21*PI()/180)</f>
-        <v>24</v>
+        <v>6.1257422745431001E-16</v>
       </c>
       <c r="H25" s="12" t="s">
         <v>32</v>
       </c>
       <c r="I25" s="13">
         <f>3*$C$25/4</f>
-        <v>72</v>
+        <v>30</v>
       </c>
       <c r="J25" s="12" t="s">
         <v>42</v>
       </c>
       <c r="K25" s="13">
         <f>3*$C$25/4</f>
-        <v>72</v>
+        <v>30</v>
       </c>
       <c r="M25" s="12" t="s">
         <v>42</v>
       </c>
       <c r="N25" s="16">
         <f>1.5*B20</f>
-        <v>36</v>
+        <v>15</v>
       </c>
     </row>
     <row r="26" spans="1:14" x14ac:dyDescent="0.25">
@@ -1908,7 +1908,7 @@
       </c>
       <c r="C26" s="3">
         <f>IF(B26=0,1,$B$20*B26)</f>
-        <v>144</v>
+        <v>60</v>
       </c>
       <c r="H26" s="12" t="s">
         <v>49</v>
@@ -1929,7 +1929,7 @@
       </c>
       <c r="N26" s="16">
         <f>(B26/2-1.5)*B20</f>
-        <v>36</v>
+        <v>15</v>
       </c>
     </row>
     <row r="27" spans="1:14" x14ac:dyDescent="0.25">
@@ -1938,28 +1938,28 @@
       </c>
       <c r="C27" s="3">
         <f>C24*C25*C26</f>
-        <v>2654208</v>
+        <v>192000</v>
       </c>
       <c r="H27" s="12" t="s">
         <v>50</v>
       </c>
       <c r="I27">
         <f>$I$26+6*$B$20</f>
-        <v>144</v>
+        <v>60</v>
       </c>
       <c r="J27" s="12" t="s">
         <v>52</v>
       </c>
       <c r="K27">
         <f>$I$26+6*$B$20</f>
-        <v>144</v>
+        <v>60</v>
       </c>
       <c r="M27" s="12" t="s">
         <v>52</v>
       </c>
       <c r="N27" s="16">
         <f>N26+(3*B20)</f>
-        <v>108</v>
+        <v>45</v>
       </c>
     </row>
     <row r="28" spans="1:14" x14ac:dyDescent="0.25">
@@ -1968,21 +1968,21 @@
       </c>
       <c r="I28" s="13">
         <f>($I$23-$I$22+1)*2</f>
-        <v>194</v>
+        <v>82</v>
       </c>
       <c r="J28" t="s">
         <v>35</v>
       </c>
       <c r="K28" s="13">
         <f>($I$23-$I$22+1)*2</f>
-        <v>194</v>
+        <v>82</v>
       </c>
       <c r="M28" t="s">
         <v>35</v>
       </c>
       <c r="N28" s="12">
         <f>(N23-N22+1)*2</f>
-        <v>194</v>
+        <v>82</v>
       </c>
     </row>
     <row r="29" spans="1:14" x14ac:dyDescent="0.25">
@@ -1991,28 +1991,28 @@
       </c>
       <c r="C29" s="13">
         <f>(C24*C25*C26)+ (N28*N29*N30) + (N37*N38*N39) + (N46*N47*N48) + (N55*N56*N57)</f>
-        <v>163090688</v>
+        <v>12063952</v>
       </c>
       <c r="H29" t="s">
         <v>36</v>
       </c>
       <c r="I29" s="13">
         <f>($I$25-$I$24+1)*2</f>
-        <v>98</v>
+        <v>42</v>
       </c>
       <c r="J29" t="s">
         <v>36</v>
       </c>
       <c r="K29" s="13">
         <f>($I$25-$I$24+1)*2</f>
-        <v>98</v>
+        <v>42</v>
       </c>
       <c r="M29" t="s">
         <v>36</v>
       </c>
       <c r="N29" s="12">
         <f>(N25-N24+1)*2</f>
-        <v>74</v>
+        <v>32</v>
       </c>
     </row>
     <row r="30" spans="1:14" x14ac:dyDescent="0.25">
@@ -2021,21 +2021,21 @@
       </c>
       <c r="I30" s="13">
         <f>($I$27-$I$26+1)*2</f>
-        <v>290</v>
+        <v>122</v>
       </c>
       <c r="J30" s="12" t="s">
         <v>48</v>
       </c>
       <c r="K30">
         <f>($I$27-$I$26+1)*2</f>
-        <v>290</v>
+        <v>122</v>
       </c>
       <c r="M30" s="12" t="s">
         <v>48</v>
       </c>
       <c r="N30" s="12">
         <f>(N27-N26+1)*2</f>
-        <v>146</v>
+        <v>62</v>
       </c>
     </row>
     <row r="31" spans="1:14" x14ac:dyDescent="0.25">
@@ -2044,21 +2044,21 @@
       </c>
       <c r="I31" s="13">
         <f>0.5*($I$28-$B$20*2*COS($B$21*PI()/180))</f>
-        <v>73</v>
+        <v>41</v>
       </c>
       <c r="J31" t="s">
         <v>43</v>
       </c>
       <c r="K31" s="13">
         <f>($K$28/4)</f>
-        <v>48.5</v>
+        <v>20.5</v>
       </c>
       <c r="M31" t="s">
         <v>43</v>
       </c>
       <c r="N31" s="16">
         <f>(B20/4)*2</f>
-        <v>12</v>
+        <v>5</v>
       </c>
     </row>
     <row r="32" spans="1:14" x14ac:dyDescent="0.25">
@@ -2067,21 +2067,21 @@
       </c>
       <c r="I32" s="13">
         <f>0.5*($I$28-$B$20*2*SIN($B$21*PI()/180))</f>
-        <v>97</v>
+        <v>31</v>
       </c>
       <c r="J32" t="s">
         <v>39</v>
       </c>
       <c r="K32" s="13">
         <f>(3*$K$28/4)</f>
-        <v>145.5</v>
+        <v>61.5</v>
       </c>
       <c r="M32" t="s">
         <v>39</v>
       </c>
       <c r="N32" s="16">
         <f>N31+(3.25*B20*2)</f>
-        <v>168</v>
+        <v>70</v>
       </c>
     </row>
     <row r="33" spans="8:14" x14ac:dyDescent="0.25">
@@ -2090,14 +2090,14 @@
       </c>
       <c r="I33" s="13">
         <f>I30/2</f>
-        <v>145</v>
+        <v>61</v>
       </c>
       <c r="J33" s="12" t="s">
         <v>44</v>
       </c>
       <c r="K33" s="13">
         <f>($K$29/4)</f>
-        <v>24.5</v>
+        <v>10.5</v>
       </c>
       <c r="M33" s="12" t="s">
         <v>44</v>
@@ -2112,21 +2112,21 @@
       </c>
       <c r="I34" s="13">
         <f>$B$20*2*COS($B$21*PI()/180)</f>
-        <v>48</v>
+        <v>1.22514845490862E-15</v>
       </c>
       <c r="J34" s="12" t="s">
         <v>45</v>
       </c>
       <c r="K34" s="13">
         <f>(3*$K$29/4)</f>
-        <v>73.5</v>
+        <v>31.5</v>
       </c>
       <c r="M34" s="12" t="s">
         <v>45</v>
       </c>
       <c r="N34" s="16">
         <f>N33+(1.25*B20*2)</f>
-        <v>60</v>
+        <v>25</v>
       </c>
     </row>
     <row r="35" spans="8:14" x14ac:dyDescent="0.25">
@@ -2136,14 +2136,14 @@
       </c>
       <c r="K35">
         <f>$B$20*2</f>
-        <v>48</v>
+        <v>20</v>
       </c>
       <c r="M35" s="12" t="s">
         <v>53</v>
       </c>
       <c r="N35" s="16">
         <f>(B20/4)*2</f>
-        <v>12</v>
+        <v>5</v>
       </c>
     </row>
     <row r="36" spans="8:14" x14ac:dyDescent="0.25">
@@ -2152,14 +2152,14 @@
       </c>
       <c r="K36">
         <f>K35+(5*B20*2)</f>
-        <v>288</v>
+        <v>120</v>
       </c>
       <c r="M36" s="12" t="s">
         <v>54</v>
       </c>
       <c r="N36" s="16">
         <f>N35+(2.5*B20*2)</f>
-        <v>132</v>
+        <v>55</v>
       </c>
     </row>
     <row r="37" spans="8:14" x14ac:dyDescent="0.25">
@@ -2168,14 +2168,14 @@
       </c>
       <c r="K37" s="13">
         <f>($K$32-$K$31+1)*2</f>
-        <v>196</v>
+        <v>84</v>
       </c>
       <c r="M37" t="s">
         <v>46</v>
       </c>
       <c r="N37" s="12">
         <f>(N32-N31+1)*2</f>
-        <v>314</v>
+        <v>132</v>
       </c>
     </row>
     <row r="38" spans="8:14" x14ac:dyDescent="0.25">
@@ -2184,14 +2184,14 @@
       </c>
       <c r="K38" s="13">
         <f>($K$34-$K$33+1)*2</f>
-        <v>100</v>
+        <v>44</v>
       </c>
       <c r="M38" t="s">
         <v>47</v>
       </c>
       <c r="N38" s="12">
         <f>(N34-N33+1)*2</f>
-        <v>122</v>
+        <v>52</v>
       </c>
     </row>
     <row r="39" spans="8:14" x14ac:dyDescent="0.25">
@@ -2200,14 +2200,14 @@
       </c>
       <c r="K39" s="13">
         <f>($K$36-$K$35+1)*2</f>
-        <v>482</v>
+        <v>202</v>
       </c>
       <c r="M39" s="12" t="s">
         <v>55</v>
       </c>
       <c r="N39" s="12">
         <f>(N36-N35+1)*2</f>
-        <v>242</v>
+        <v>102</v>
       </c>
     </row>
     <row r="40" spans="8:14" x14ac:dyDescent="0.25">
@@ -2216,14 +2216,14 @@
       </c>
       <c r="K40" s="13">
         <f>0.5*($K$37-$B$20*4*COS($B$21*PI()/180))</f>
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="M40" t="s">
         <v>59</v>
       </c>
       <c r="N40" s="16">
         <f>(B20/4)*4</f>
-        <v>24</v>
+        <v>10</v>
       </c>
     </row>
     <row r="41" spans="8:14" x14ac:dyDescent="0.25">
@@ -2232,14 +2232,14 @@
       </c>
       <c r="K41" s="13">
         <f>0.5*($K$38-$B$20*4*SIN($B$21*PI()/180))</f>
-        <v>50</v>
+        <v>2</v>
       </c>
       <c r="M41" t="s">
         <v>60</v>
       </c>
       <c r="N41" s="16">
         <f>N40+(2.5*B20*4)</f>
-        <v>264</v>
+        <v>110</v>
       </c>
     </row>
     <row r="42" spans="8:14" x14ac:dyDescent="0.25">
@@ -2248,7 +2248,7 @@
       </c>
       <c r="K42" s="13">
         <f>K39/2</f>
-        <v>241</v>
+        <v>101</v>
       </c>
       <c r="M42" s="12" t="s">
         <v>61</v>
@@ -2263,14 +2263,14 @@
       </c>
       <c r="K43" s="13">
         <f>$B$20*4*COS($B$21*PI()/180)</f>
-        <v>96</v>
+        <v>2.45029690981724E-15</v>
       </c>
       <c r="M43" s="12" t="s">
         <v>62</v>
       </c>
       <c r="N43" s="16">
         <f>B20*4</f>
-        <v>96</v>
+        <v>40</v>
       </c>
     </row>
     <row r="44" spans="8:14" x14ac:dyDescent="0.25">
@@ -2279,7 +2279,7 @@
       </c>
       <c r="N44" s="16">
         <f>(B20/4)*4</f>
-        <v>24</v>
+        <v>10</v>
       </c>
     </row>
     <row r="45" spans="8:14" x14ac:dyDescent="0.25">
@@ -2288,7 +2288,7 @@
       </c>
       <c r="N45" s="16">
         <f>N44+(2*B20*4)</f>
-        <v>216</v>
+        <v>90</v>
       </c>
     </row>
     <row r="46" spans="8:14" x14ac:dyDescent="0.25">
@@ -2297,7 +2297,7 @@
       </c>
       <c r="N46" s="12">
         <f>(N41-N40+1)*2</f>
-        <v>482</v>
+        <v>202</v>
       </c>
     </row>
     <row r="47" spans="8:14" x14ac:dyDescent="0.25">
@@ -2306,7 +2306,7 @@
       </c>
       <c r="N47" s="12">
         <f>(N43-N42+1)*2</f>
-        <v>194</v>
+        <v>82</v>
       </c>
     </row>
     <row r="48" spans="8:14" x14ac:dyDescent="0.25">
@@ -2315,7 +2315,7 @@
       </c>
       <c r="N48" s="12">
         <f>(N45-N44+1)*2</f>
-        <v>386</v>
+        <v>162</v>
       </c>
     </row>
     <row r="49" spans="13:14" x14ac:dyDescent="0.25">
@@ -2324,7 +2324,7 @@
       </c>
       <c r="N49" s="16">
         <f>(B20/4)*8</f>
-        <v>48</v>
+        <v>20</v>
       </c>
     </row>
     <row r="50" spans="13:14" x14ac:dyDescent="0.25">
@@ -2333,7 +2333,7 @@
       </c>
       <c r="N50" s="16">
         <f>N49+(1.75*B20*8)</f>
-        <v>384</v>
+        <v>160</v>
       </c>
     </row>
     <row r="51" spans="13:14" x14ac:dyDescent="0.25">
@@ -2350,7 +2350,7 @@
       </c>
       <c r="N52" s="16">
         <f>0.75*B20*8</f>
-        <v>144</v>
+        <v>60</v>
       </c>
     </row>
     <row r="53" spans="13:14" x14ac:dyDescent="0.25">
@@ -2359,7 +2359,7 @@
       </c>
       <c r="N53" s="16">
         <f>(B20/4)*8</f>
-        <v>48</v>
+        <v>20</v>
       </c>
     </row>
     <row r="54" spans="13:14" x14ac:dyDescent="0.25">
@@ -2368,7 +2368,7 @@
       </c>
       <c r="N54" s="16">
         <f>N53+(1.5*B20*8)</f>
-        <v>336</v>
+        <v>140</v>
       </c>
     </row>
     <row r="55" spans="13:14" x14ac:dyDescent="0.25">
@@ -2377,7 +2377,7 @@
       </c>
       <c r="N55" s="12">
         <f>(N50-N49+1)*2</f>
-        <v>674</v>
+        <v>282</v>
       </c>
     </row>
     <row r="56" spans="13:14" x14ac:dyDescent="0.25">
@@ -2386,7 +2386,7 @@
       </c>
       <c r="N56" s="12">
         <f>(N52-N51+1)*2</f>
-        <v>290</v>
+        <v>122</v>
       </c>
     </row>
     <row r="57" spans="13:14" x14ac:dyDescent="0.25">
@@ -2395,7 +2395,7 @@
       </c>
       <c r="N57" s="12">
         <f>(N54-N53+1)*2</f>
-        <v>578</v>
+        <v>242</v>
       </c>
     </row>
     <row r="58" spans="13:14" x14ac:dyDescent="0.25">
@@ -2404,7 +2404,7 @@
       </c>
       <c r="N58" s="16">
         <f>(B20/4)*16</f>
-        <v>96</v>
+        <v>40</v>
       </c>
     </row>
     <row r="59" spans="13:14" x14ac:dyDescent="0.25">
@@ -2421,7 +2421,7 @@
       </c>
       <c r="N60" s="16">
         <f>N57/2</f>
-        <v>289</v>
+        <v>121</v>
       </c>
     </row>
     <row r="61" spans="13:14" x14ac:dyDescent="0.25">
@@ -2430,7 +2430,7 @@
       </c>
       <c r="N61" s="16">
         <f>B20*16</f>
-        <v>384</v>
+        <v>160</v>
       </c>
     </row>
   </sheetData>
@@ -2456,7 +2456,7 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:N61"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView topLeftCell="A15" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Changed is_nan() def and added extrapolation
</commit_message>
<xml_diff>
--- a/LUMA/tools/SizingGuide.xlsx
+++ b/LUMA/tools/SizingGuide.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="16925"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17127"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Adrian\Dropbox (Personal)\0. Work\3. LBM\C++ Projects\LUMA\LUMA\tools\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dropbox (CFDTM)\0. Work\3. LBM\C++ Projects\LUMA\LUMA\tools\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9372" tabRatio="573"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9372" tabRatio="573" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Archer" sheetId="11" r:id="rId1"/>
@@ -813,8 +813,8 @@
   <sheetPr codeName="Sheet4"/>
   <dimension ref="A1:N61"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B22" sqref="B22"/>
+    <sheetView topLeftCell="A13" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -880,10 +880,10 @@
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="4">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="B2" s="4">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C2" s="4">
         <v>6</v>
@@ -898,11 +898,11 @@
       </c>
       <c r="F2" s="5">
         <f t="shared" ref="F2:F16" si="2">($C$24/A2)+2</f>
-        <v>22</v>
+        <v>12</v>
       </c>
       <c r="G2" s="5">
         <f t="shared" ref="G2:G16" si="3">($C$25/B2)+2</f>
-        <v>12</v>
+        <v>22</v>
       </c>
       <c r="H2" s="5">
         <f t="shared" ref="H2:H16" si="4">($C$26/C2)+2</f>
@@ -1826,7 +1826,7 @@
         <v>8</v>
       </c>
       <c r="C24" s="3">
-        <f>$B$20*B24</f>
+        <f>B20*B24</f>
         <v>80</v>
       </c>
       <c r="E24" s="12"/>
@@ -1866,7 +1866,7 @@
         <v>4</v>
       </c>
       <c r="C25" s="3">
-        <f t="shared" ref="C25" si="12">$B$20*B25</f>
+        <f>B20*B25</f>
         <v>40</v>
       </c>
       <c r="E25" s="12"/>
@@ -1907,7 +1907,7 @@
         <v>6</v>
       </c>
       <c r="C26" s="3">
-        <f>IF(B26=0,1,$B$20*B26)</f>
+        <f>B20*B26</f>
         <v>60</v>
       </c>
       <c r="H26" s="12" t="s">
@@ -2456,8 +2456,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:N61"/>
   <sheetViews>
-    <sheetView topLeftCell="A15" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5:C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -2541,31 +2541,31 @@
       </c>
       <c r="F2" s="5">
         <f t="shared" ref="F2:F16" si="2">($C$24/A2)+2</f>
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="G2" s="5">
         <f t="shared" ref="G2:G16" si="3">($C$25/B2)+2</f>
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="H2" s="5">
         <f t="shared" ref="H2:H16" si="4">($C$26/C2)+2</f>
-        <v>17</v>
+        <v>32</v>
       </c>
       <c r="I2" s="5">
         <f t="shared" ref="I2:I16" si="5">F2*G2*H2</f>
-        <v>833</v>
+        <v>4608</v>
       </c>
       <c r="J2" s="5">
         <f t="shared" ref="J2:J16" si="6">4*F2*G2+4*G2*H2+4*F2*H2</f>
-        <v>1148</v>
+        <v>3648</v>
       </c>
       <c r="K2" s="5">
         <f t="shared" ref="K2:K16" si="7">J2*E2</f>
-        <v>73472</v>
+        <v>233472</v>
       </c>
       <c r="L2" s="5">
         <f t="shared" ref="L2:L16" si="8">K2/$C$27*100</f>
-        <v>306.13333333333333</v>
+        <v>121.6</v>
       </c>
       <c r="M2" s="6" t="b">
         <f>IF((F2-FLOOR(F2,1))=0,IF((G2-FLOOR(G2,1))=0,IF((H2-FLOOR(H2,1))=0,TRUE,FALSE),FALSE),FALSE)</f>
@@ -2596,35 +2596,35 @@
       </c>
       <c r="F3" s="5">
         <f t="shared" si="2"/>
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="G3" s="5">
         <f t="shared" si="3"/>
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="H3" s="5">
         <f t="shared" si="4"/>
-        <v>9.5</v>
+        <v>17</v>
       </c>
       <c r="I3" s="5">
         <f t="shared" si="5"/>
-        <v>465.5</v>
+        <v>2448</v>
       </c>
       <c r="J3" s="5">
         <f t="shared" si="6"/>
-        <v>728</v>
+        <v>2208</v>
       </c>
       <c r="K3" s="5">
         <f t="shared" si="7"/>
-        <v>93184</v>
+        <v>282624</v>
       </c>
       <c r="L3" s="5">
         <f t="shared" si="8"/>
-        <v>388.26666666666665</v>
+        <v>147.19999999999999</v>
       </c>
       <c r="M3" s="6" t="b">
         <f>IF((F3-FLOOR(F3,1))=0,IF((G3-FLOOR(G3,1))=0,IF((H3-FLOOR(H3,1))=0,TRUE,FALSE),FALSE),FALSE)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N3" s="6" t="b">
         <f t="shared" ref="N3:N16" si="9">IF(($D3-FLOOR($D3,1))=0,TRUE,FALSE)</f>
@@ -2651,31 +2651,31 @@
       </c>
       <c r="F4" s="5">
         <f t="shared" si="2"/>
-        <v>5.3333333333333339</v>
+        <v>8.6666666666666679</v>
       </c>
       <c r="G4" s="5">
         <f t="shared" si="3"/>
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="H4" s="5">
         <f t="shared" si="4"/>
-        <v>9.5</v>
+        <v>17</v>
       </c>
       <c r="I4" s="5">
         <f t="shared" si="5"/>
-        <v>354.66666666666669</v>
+        <v>1768.0000000000002</v>
       </c>
       <c r="J4" s="5">
         <f t="shared" si="6"/>
-        <v>618</v>
+        <v>1821.3333333333335</v>
       </c>
       <c r="K4" s="5">
         <f t="shared" si="7"/>
-        <v>118656</v>
+        <v>349696</v>
       </c>
       <c r="L4" s="5">
         <f t="shared" si="8"/>
-        <v>494.4</v>
+        <v>182.13333333333333</v>
       </c>
       <c r="M4" s="6" t="b">
         <f t="shared" ref="M4:M6" si="10">IF((F4-FLOOR(F4,1))=0,IF((G4-FLOOR(G4,1))=0,IF((H4-FLOOR(H4,1))=0,TRUE,FALSE),FALSE),FALSE)</f>
@@ -2706,31 +2706,31 @@
       </c>
       <c r="F5" s="5">
         <f t="shared" si="2"/>
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="G5" s="5">
         <f t="shared" si="3"/>
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="H5" s="5">
         <f t="shared" si="4"/>
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="I5" s="5">
         <f t="shared" si="5"/>
-        <v>343</v>
+        <v>1728</v>
       </c>
       <c r="J5" s="5">
         <f t="shared" si="6"/>
-        <v>588</v>
+        <v>1728</v>
       </c>
       <c r="K5" s="5">
         <f t="shared" si="7"/>
-        <v>112896</v>
+        <v>331776</v>
       </c>
       <c r="L5" s="5">
         <f t="shared" si="8"/>
-        <v>470.4</v>
+        <v>172.8</v>
       </c>
       <c r="M5" s="6" t="b">
         <f t="shared" si="10"/>
@@ -2761,35 +2761,35 @@
       </c>
       <c r="F6" s="5">
         <f t="shared" si="2"/>
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="G6" s="5">
         <f t="shared" si="3"/>
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="H6" s="5">
         <f t="shared" si="4"/>
-        <v>9.5</v>
+        <v>17</v>
       </c>
       <c r="I6" s="5">
         <f t="shared" si="5"/>
-        <v>266</v>
+        <v>1224</v>
       </c>
       <c r="J6" s="5">
         <f t="shared" si="6"/>
-        <v>530</v>
+        <v>1512</v>
       </c>
       <c r="K6" s="5">
         <f t="shared" si="7"/>
-        <v>169600</v>
+        <v>483840</v>
       </c>
       <c r="L6" s="5">
         <f t="shared" si="8"/>
-        <v>706.66666666666663</v>
+        <v>252</v>
       </c>
       <c r="M6" s="6" t="b">
         <f t="shared" si="10"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N6" s="6" t="b">
         <f t="shared" si="9"/>
@@ -2816,31 +2816,31 @@
       </c>
       <c r="F7" s="5">
         <f t="shared" si="2"/>
-        <v>12</v>
+        <v>22</v>
       </c>
       <c r="G7" s="5">
         <f t="shared" si="3"/>
-        <v>4.2222222222222223</v>
+        <v>6.4444444444444446</v>
       </c>
       <c r="H7" s="5">
         <f t="shared" si="4"/>
-        <v>9.5</v>
+        <v>17</v>
       </c>
       <c r="I7" s="5">
         <f t="shared" si="5"/>
-        <v>481.33333333333337</v>
+        <v>2410.2222222222222</v>
       </c>
       <c r="J7" s="5">
         <f t="shared" si="6"/>
-        <v>819.11111111111109</v>
+        <v>2501.333333333333</v>
       </c>
       <c r="K7" s="5">
         <f t="shared" si="7"/>
-        <v>117952</v>
+        <v>360191.99999999994</v>
       </c>
       <c r="L7" s="5">
         <f t="shared" si="8"/>
-        <v>491.46666666666664</v>
+        <v>187.59999999999997</v>
       </c>
       <c r="M7" s="6" t="b">
         <f>IF((F7-FLOOR(F7,1))=0,IF((G7-FLOOR(G7,1))=0,IF((H7-FLOOR(H7,1))=0,TRUE,FALSE),FALSE),FALSE)</f>
@@ -2871,35 +2871,35 @@
       </c>
       <c r="F8" s="5">
         <f t="shared" si="2"/>
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="G8" s="5">
         <f t="shared" si="3"/>
-        <v>4.5</v>
+        <v>7</v>
       </c>
       <c r="H8" s="5">
         <f t="shared" si="4"/>
-        <v>32</v>
+        <v>62</v>
       </c>
       <c r="I8" s="5">
         <f t="shared" si="5"/>
-        <v>1008</v>
+        <v>5208</v>
       </c>
       <c r="J8" s="5">
         <f t="shared" si="6"/>
-        <v>1598</v>
+        <v>5048</v>
       </c>
       <c r="K8" s="5">
         <f t="shared" si="7"/>
-        <v>102272</v>
+        <v>323072</v>
       </c>
       <c r="L8" s="5">
         <f t="shared" si="8"/>
-        <v>426.13333333333333</v>
+        <v>168.26666666666668</v>
       </c>
       <c r="M8" s="6" t="b">
         <f t="shared" ref="M8:M16" si="11">IF((F8-FLOOR(F8,1))=0,IF((G8-FLOOR(G8,1))=0,IF((H8-FLOOR(H8,1))=0,TRUE,FALSE),FALSE),FALSE)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N8" s="6" t="b">
         <f t="shared" si="9"/>
@@ -2926,35 +2926,35 @@
       </c>
       <c r="F9" s="5">
         <f t="shared" si="2"/>
-        <v>4.5</v>
+        <v>7</v>
       </c>
       <c r="G9" s="5">
         <f t="shared" si="3"/>
-        <v>4.5</v>
+        <v>7</v>
       </c>
       <c r="H9" s="5">
         <f t="shared" si="4"/>
-        <v>32</v>
+        <v>62</v>
       </c>
       <c r="I9" s="5">
         <f t="shared" si="5"/>
-        <v>648</v>
+        <v>3038</v>
       </c>
       <c r="J9" s="5">
         <f t="shared" si="6"/>
-        <v>1233</v>
+        <v>3668</v>
       </c>
       <c r="K9" s="5">
         <f t="shared" si="7"/>
-        <v>157824</v>
+        <v>469504</v>
       </c>
       <c r="L9" s="5">
         <f t="shared" si="8"/>
-        <v>657.59999999999991</v>
+        <v>244.5333333333333</v>
       </c>
       <c r="M9" s="6" t="b">
         <f t="shared" si="11"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N9" s="6" t="b">
         <f t="shared" si="9"/>
@@ -2981,31 +2981,31 @@
       </c>
       <c r="F10" s="5">
         <f t="shared" si="2"/>
-        <v>3.666666666666667</v>
+        <v>5.3333333333333339</v>
       </c>
       <c r="G10" s="5">
         <f t="shared" si="3"/>
-        <v>4.5</v>
+        <v>7</v>
       </c>
       <c r="H10" s="5">
         <f t="shared" si="4"/>
-        <v>32</v>
+        <v>62</v>
       </c>
       <c r="I10" s="5">
         <f t="shared" si="5"/>
-        <v>528</v>
+        <v>2314.666666666667</v>
       </c>
       <c r="J10" s="5">
         <f t="shared" si="6"/>
-        <v>1111.3333333333335</v>
+        <v>3208</v>
       </c>
       <c r="K10" s="5">
         <f t="shared" si="7"/>
-        <v>213376.00000000003</v>
+        <v>615936</v>
       </c>
       <c r="L10" s="5">
         <f t="shared" si="8"/>
-        <v>889.06666666666683</v>
+        <v>320.8</v>
       </c>
       <c r="M10" s="6" t="b">
         <f t="shared" si="11"/>
@@ -3036,31 +3036,31 @@
       </c>
       <c r="F11" s="5">
         <f t="shared" si="2"/>
-        <v>3.25</v>
+        <v>4.5</v>
       </c>
       <c r="G11" s="5">
         <f t="shared" si="3"/>
-        <v>4.5</v>
+        <v>7</v>
       </c>
       <c r="H11" s="5">
         <f t="shared" si="4"/>
-        <v>32</v>
+        <v>62</v>
       </c>
       <c r="I11" s="5">
         <f t="shared" si="5"/>
-        <v>468</v>
+        <v>1953</v>
       </c>
       <c r="J11" s="5">
         <f t="shared" si="6"/>
-        <v>1050.5</v>
+        <v>2978</v>
       </c>
       <c r="K11" s="5">
         <f t="shared" si="7"/>
-        <v>268928</v>
+        <v>762368</v>
       </c>
       <c r="L11" s="5">
         <f t="shared" si="8"/>
-        <v>1120.5333333333333</v>
+        <v>397.06666666666666</v>
       </c>
       <c r="M11" s="6" t="b">
         <f t="shared" si="11"/>
@@ -3091,35 +3091,35 @@
       </c>
       <c r="F12" s="5">
         <f t="shared" si="2"/>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="G12" s="5">
         <f t="shared" si="3"/>
-        <v>4.5</v>
+        <v>7</v>
       </c>
       <c r="H12" s="5">
         <f t="shared" si="4"/>
-        <v>32</v>
+        <v>62</v>
       </c>
       <c r="I12" s="5">
         <f t="shared" si="5"/>
-        <v>432</v>
+        <v>1736</v>
       </c>
       <c r="J12" s="5">
         <f t="shared" si="6"/>
-        <v>1014</v>
+        <v>2840</v>
       </c>
       <c r="K12" s="5">
         <f t="shared" si="7"/>
-        <v>324480</v>
+        <v>908800</v>
       </c>
       <c r="L12" s="5">
         <f t="shared" si="8"/>
-        <v>1352</v>
+        <v>473.33333333333331</v>
       </c>
       <c r="M12" s="6" t="b">
         <f t="shared" si="11"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N12" s="6" t="b">
         <f t="shared" si="9"/>
@@ -3146,31 +3146,31 @@
       </c>
       <c r="F13" s="5">
         <f t="shared" si="2"/>
-        <v>4.5</v>
+        <v>7</v>
       </c>
       <c r="G13" s="5">
         <f t="shared" si="3"/>
-        <v>4.2222222222222223</v>
+        <v>6.4444444444444446</v>
       </c>
       <c r="H13" s="5">
         <f t="shared" si="4"/>
-        <v>9.5</v>
+        <v>17</v>
       </c>
       <c r="I13" s="5">
         <f t="shared" si="5"/>
-        <v>180.5</v>
+        <v>766.88888888888891</v>
       </c>
       <c r="J13" s="5">
         <f t="shared" si="6"/>
-        <v>407.44444444444446</v>
+        <v>1094.6666666666667</v>
       </c>
       <c r="K13" s="5">
         <f t="shared" si="7"/>
-        <v>234688</v>
+        <v>630528</v>
       </c>
       <c r="L13" s="5">
         <f t="shared" si="8"/>
-        <v>977.86666666666656</v>
+        <v>328.4</v>
       </c>
       <c r="M13" s="6" t="b">
         <f t="shared" si="11"/>
@@ -3201,31 +3201,31 @@
       </c>
       <c r="F14" s="5">
         <f t="shared" si="2"/>
-        <v>12</v>
+        <v>22</v>
       </c>
       <c r="G14" s="5">
         <f t="shared" si="3"/>
-        <v>12</v>
+        <v>22</v>
       </c>
       <c r="H14" s="5">
         <f t="shared" si="4"/>
-        <v>17</v>
+        <v>32</v>
       </c>
       <c r="I14" s="5">
         <f t="shared" si="5"/>
-        <v>2448</v>
+        <v>15488</v>
       </c>
       <c r="J14" s="5">
         <f t="shared" si="6"/>
-        <v>2208</v>
+        <v>7568</v>
       </c>
       <c r="K14" s="5">
         <f t="shared" si="7"/>
-        <v>35328</v>
+        <v>121088</v>
       </c>
       <c r="L14" s="5">
         <f t="shared" si="8"/>
-        <v>147.19999999999999</v>
+        <v>63.06666666666667</v>
       </c>
       <c r="M14" s="6" t="b">
         <f t="shared" si="11"/>
@@ -3256,31 +3256,31 @@
       </c>
       <c r="F15" s="5">
         <f t="shared" si="2"/>
-        <v>22</v>
+        <v>42</v>
       </c>
       <c r="G15" s="5">
         <f t="shared" si="3"/>
-        <v>12</v>
+        <v>22</v>
       </c>
       <c r="H15" s="5">
         <f t="shared" si="4"/>
-        <v>17</v>
+        <v>32</v>
       </c>
       <c r="I15" s="5">
         <f t="shared" si="5"/>
-        <v>4488</v>
+        <v>29568</v>
       </c>
       <c r="J15" s="5">
         <f t="shared" si="6"/>
-        <v>3368</v>
+        <v>11888</v>
       </c>
       <c r="K15" s="5">
         <f t="shared" si="7"/>
-        <v>26944</v>
+        <v>95104</v>
       </c>
       <c r="L15" s="5">
         <f t="shared" si="8"/>
-        <v>112.26666666666667</v>
+        <v>49.533333333333331</v>
       </c>
       <c r="M15" s="6" t="b">
         <f t="shared" si="11"/>
@@ -3311,31 +3311,31 @@
       </c>
       <c r="F16" s="5">
         <f t="shared" si="2"/>
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="G16" s="5">
         <f t="shared" si="3"/>
-        <v>4.5</v>
+        <v>7</v>
       </c>
       <c r="H16" s="5">
         <f t="shared" si="4"/>
-        <v>5.75</v>
+        <v>9.5</v>
       </c>
       <c r="I16" s="5">
         <f t="shared" si="5"/>
-        <v>155.25</v>
+        <v>665</v>
       </c>
       <c r="J16" s="5">
         <f t="shared" si="6"/>
-        <v>349.5</v>
+        <v>926</v>
       </c>
       <c r="K16" s="5">
         <f t="shared" si="7"/>
-        <v>223680</v>
+        <v>592640</v>
       </c>
       <c r="L16" s="5">
         <f t="shared" si="8"/>
-        <v>932</v>
+        <v>308.66666666666663</v>
       </c>
       <c r="M16" s="6" t="b">
         <f t="shared" si="11"/>
@@ -3362,7 +3362,7 @@
         <v>10</v>
       </c>
       <c r="B20">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="D20" s="10" t="s">
         <v>18</v>
@@ -3382,7 +3382,7 @@
       </c>
       <c r="N22" s="16">
         <f>0.25*(B24-4)*B20</f>
-        <v>5</v>
+        <v>10</v>
       </c>
     </row>
     <row r="23" spans="1:14" x14ac:dyDescent="0.25">
@@ -3398,7 +3398,7 @@
       </c>
       <c r="N23" s="16">
         <f>N22+(4*B20)</f>
-        <v>25</v>
+        <v>50</v>
       </c>
     </row>
     <row r="24" spans="1:14" x14ac:dyDescent="0.25">
@@ -3410,7 +3410,7 @@
       </c>
       <c r="C24" s="3">
         <f>$B$20*B24</f>
-        <v>40</v>
+        <v>80</v>
       </c>
       <c r="E24" s="12"/>
       <c r="H24" s="12"/>
@@ -3431,7 +3431,7 @@
       </c>
       <c r="C25" s="3">
         <f t="shared" ref="C25:C26" si="12">$B$20*B25</f>
-        <v>20</v>
+        <v>40</v>
       </c>
       <c r="E25" s="12"/>
       <c r="H25" s="12"/>
@@ -3441,7 +3441,7 @@
       </c>
       <c r="N25" s="16">
         <f>1.5*B20</f>
-        <v>7.5</v>
+        <v>15</v>
       </c>
     </row>
     <row r="26" spans="1:14" x14ac:dyDescent="0.25">
@@ -3453,7 +3453,7 @@
       </c>
       <c r="C26" s="3">
         <f t="shared" si="12"/>
-        <v>30</v>
+        <v>60</v>
       </c>
       <c r="J26" s="12"/>
       <c r="M26" s="12" t="s">
@@ -3461,7 +3461,7 @@
       </c>
       <c r="N26" s="16">
         <f>((B26/2-1.5)*B20) - 1</f>
-        <v>6.5</v>
+        <v>14</v>
       </c>
     </row>
     <row r="27" spans="1:14" x14ac:dyDescent="0.25">
@@ -3470,7 +3470,7 @@
       </c>
       <c r="C27" s="3">
         <f>C24*C25*C26</f>
-        <v>24000</v>
+        <v>192000</v>
       </c>
       <c r="H27" s="12"/>
       <c r="J27" s="12"/>
@@ -3479,7 +3479,7 @@
       </c>
       <c r="N27" s="16">
         <f>N26+(3*B20)</f>
-        <v>21.5</v>
+        <v>44</v>
       </c>
     </row>
     <row r="28" spans="1:14" x14ac:dyDescent="0.25">
@@ -3490,7 +3490,7 @@
       </c>
       <c r="N28" s="12">
         <f>(N23-N22+1)*2</f>
-        <v>42</v>
+        <v>82</v>
       </c>
     </row>
     <row r="29" spans="1:14" x14ac:dyDescent="0.25">
@@ -3499,7 +3499,7 @@
       </c>
       <c r="C29" s="13">
         <f>(C24*C25*C26)+ (N28*N29*N30) + (N37*N38*N39) + (N46*N47*N48) + (N55*N56*N57)</f>
-        <v>1566292</v>
+        <v>12063952</v>
       </c>
       <c r="J29" s="12"/>
       <c r="M29" t="s">
@@ -3507,7 +3507,7 @@
       </c>
       <c r="N29" s="12">
         <f>(N25-N24+1)*2</f>
-        <v>17</v>
+        <v>32</v>
       </c>
     </row>
     <row r="30" spans="1:14" x14ac:dyDescent="0.25">
@@ -3518,7 +3518,7 @@
       </c>
       <c r="N30" s="12">
         <f>(N27-N26+1)*2</f>
-        <v>32</v>
+        <v>62</v>
       </c>
     </row>
     <row r="31" spans="1:14" x14ac:dyDescent="0.25">
@@ -3529,7 +3529,7 @@
       </c>
       <c r="N31" s="16">
         <f>(B20/4)*2</f>
-        <v>2.5</v>
+        <v>5</v>
       </c>
     </row>
     <row r="32" spans="1:14" x14ac:dyDescent="0.25">
@@ -3539,7 +3539,7 @@
       </c>
       <c r="N32" s="16">
         <f>N31+(3.25*B20*2)</f>
-        <v>35</v>
+        <v>70</v>
       </c>
     </row>
     <row r="33" spans="8:14" x14ac:dyDescent="0.25">
@@ -3559,7 +3559,7 @@
       </c>
       <c r="N34" s="16">
         <f>N33+(1.25*B20*2)</f>
-        <v>12.5</v>
+        <v>25</v>
       </c>
     </row>
     <row r="35" spans="8:14" x14ac:dyDescent="0.25">
@@ -3568,7 +3568,7 @@
       </c>
       <c r="N35" s="16">
         <f>(B20/4)*2</f>
-        <v>2.5</v>
+        <v>5</v>
       </c>
     </row>
     <row r="36" spans="8:14" x14ac:dyDescent="0.25">
@@ -3577,7 +3577,7 @@
       </c>
       <c r="N36" s="16">
         <f>N35+(2.5*B20*2)</f>
-        <v>27.5</v>
+        <v>55</v>
       </c>
     </row>
     <row r="37" spans="8:14" x14ac:dyDescent="0.25">
@@ -3586,7 +3586,7 @@
       </c>
       <c r="N37" s="12">
         <f>(N32-N31+1)*2</f>
-        <v>67</v>
+        <v>132</v>
       </c>
     </row>
     <row r="38" spans="8:14" x14ac:dyDescent="0.25">
@@ -3595,7 +3595,7 @@
       </c>
       <c r="N38" s="12">
         <f>(N34-N33+1)*2</f>
-        <v>27</v>
+        <v>52</v>
       </c>
     </row>
     <row r="39" spans="8:14" x14ac:dyDescent="0.25">
@@ -3604,7 +3604,7 @@
       </c>
       <c r="N39" s="12">
         <f>(N36-N35+1)*2</f>
-        <v>52</v>
+        <v>102</v>
       </c>
     </row>
     <row r="40" spans="8:14" x14ac:dyDescent="0.25">
@@ -3613,7 +3613,7 @@
       </c>
       <c r="N40" s="16">
         <f>(B20/4)*4</f>
-        <v>5</v>
+        <v>10</v>
       </c>
     </row>
     <row r="41" spans="8:14" x14ac:dyDescent="0.25">
@@ -3622,7 +3622,7 @@
       </c>
       <c r="N41" s="16">
         <f>N40+(2.5*B20*4)</f>
-        <v>55</v>
+        <v>110</v>
       </c>
     </row>
     <row r="42" spans="8:14" x14ac:dyDescent="0.25">
@@ -3639,7 +3639,7 @@
       </c>
       <c r="N43" s="16">
         <f>B20*4</f>
-        <v>20</v>
+        <v>40</v>
       </c>
     </row>
     <row r="44" spans="8:14" x14ac:dyDescent="0.25">
@@ -3648,7 +3648,7 @@
       </c>
       <c r="N44" s="16">
         <f>(B20/4)*4</f>
-        <v>5</v>
+        <v>10</v>
       </c>
     </row>
     <row r="45" spans="8:14" x14ac:dyDescent="0.25">
@@ -3657,7 +3657,7 @@
       </c>
       <c r="N45" s="16">
         <f>N44+(2*B20*4)</f>
-        <v>45</v>
+        <v>90</v>
       </c>
     </row>
     <row r="46" spans="8:14" x14ac:dyDescent="0.25">
@@ -3666,7 +3666,7 @@
       </c>
       <c r="N46" s="12">
         <f>(N41-N40+1)*2</f>
-        <v>102</v>
+        <v>202</v>
       </c>
     </row>
     <row r="47" spans="8:14" x14ac:dyDescent="0.25">
@@ -3675,7 +3675,7 @@
       </c>
       <c r="N47" s="12">
         <f>(N43-N42+1)*2</f>
-        <v>42</v>
+        <v>82</v>
       </c>
     </row>
     <row r="48" spans="8:14" x14ac:dyDescent="0.25">
@@ -3684,7 +3684,7 @@
       </c>
       <c r="N48" s="12">
         <f>(N45-N44+1)*2</f>
-        <v>82</v>
+        <v>162</v>
       </c>
     </row>
     <row r="49" spans="13:14" x14ac:dyDescent="0.25">
@@ -3693,7 +3693,7 @@
       </c>
       <c r="N49" s="16">
         <f>(B20/4)*8</f>
-        <v>10</v>
+        <v>20</v>
       </c>
     </row>
     <row r="50" spans="13:14" x14ac:dyDescent="0.25">
@@ -3702,7 +3702,7 @@
       </c>
       <c r="N50" s="16">
         <f>N49+(1.75*B20*8)</f>
-        <v>80</v>
+        <v>160</v>
       </c>
     </row>
     <row r="51" spans="13:14" x14ac:dyDescent="0.25">
@@ -3719,7 +3719,7 @@
       </c>
       <c r="N52" s="16">
         <f>0.75*B20*8</f>
-        <v>30</v>
+        <v>60</v>
       </c>
     </row>
     <row r="53" spans="13:14" x14ac:dyDescent="0.25">
@@ -3728,7 +3728,7 @@
       </c>
       <c r="N53" s="16">
         <f>(B20/4)*8</f>
-        <v>10</v>
+        <v>20</v>
       </c>
     </row>
     <row r="54" spans="13:14" x14ac:dyDescent="0.25">
@@ -3737,7 +3737,7 @@
       </c>
       <c r="N54" s="16">
         <f>N53+(1.5*B20*8)</f>
-        <v>70</v>
+        <v>140</v>
       </c>
     </row>
     <row r="55" spans="13:14" x14ac:dyDescent="0.25">
@@ -3746,7 +3746,7 @@
       </c>
       <c r="N55" s="12">
         <f>(N50-N49+1)*2</f>
-        <v>142</v>
+        <v>282</v>
       </c>
     </row>
     <row r="56" spans="13:14" x14ac:dyDescent="0.25">
@@ -3755,7 +3755,7 @@
       </c>
       <c r="N56" s="12">
         <f>(N52-N51+1)*2</f>
-        <v>62</v>
+        <v>122</v>
       </c>
     </row>
     <row r="57" spans="13:14" x14ac:dyDescent="0.25">
@@ -3764,7 +3764,7 @@
       </c>
       <c r="N57" s="12">
         <f>(N54-N53+1)*2</f>
-        <v>122</v>
+        <v>242</v>
       </c>
     </row>
     <row r="58" spans="13:14" x14ac:dyDescent="0.25">
@@ -3773,7 +3773,7 @@
       </c>
       <c r="N58" s="16">
         <f>(B20/4)*16</f>
-        <v>20</v>
+        <v>40</v>
       </c>
     </row>
     <row r="59" spans="13:14" x14ac:dyDescent="0.25">
@@ -3790,7 +3790,7 @@
       </c>
       <c r="N60" s="16">
         <f>N57/2</f>
-        <v>61</v>
+        <v>121</v>
       </c>
     </row>
     <row r="61" spans="13:14" x14ac:dyDescent="0.25">
@@ -3799,7 +3799,7 @@
       </c>
       <c r="N61" s="16">
         <f>B20*16</f>
-        <v>80</v>
+        <v>160</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Changes to ASCII dump to match LUMIS,IBM init fix,new vtk merge tool, tool upgrades
</commit_message>
<xml_diff>
--- a/LUMA/tools/SizingGuide.xlsx
+++ b/LUMA/tools/SizingGuide.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="317" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="317" uniqueCount="81">
   <si>
     <t>No of Nodes</t>
   </si>
@@ -273,6 +273,9 @@
   <si>
     <t>Points 
 per L</t>
+  </si>
+  <si>
+    <t>D</t>
   </si>
 </sst>
 </file>
@@ -2457,7 +2460,7 @@
   <dimension ref="A1:N61"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5:C5"/>
+      <selection activeCell="G19" sqref="G19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -2523,49 +2526,49 @@
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="4">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="B2" s="4">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C2" s="4">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D2" s="5">
         <f t="shared" ref="D2:D16" si="0">E2/$B$19</f>
-        <v>1</v>
+        <v>6.25E-2</v>
       </c>
       <c r="E2" s="5">
         <f t="shared" ref="E2:E16" si="1">A2*B2*C2</f>
-        <v>64</v>
+        <v>4</v>
       </c>
       <c r="F2" s="5">
         <f t="shared" ref="F2:F16" si="2">($C$24/A2)+2</f>
-        <v>12</v>
+        <v>202</v>
       </c>
       <c r="G2" s="5">
         <f t="shared" ref="G2:G16" si="3">($C$25/B2)+2</f>
-        <v>12</v>
+        <v>202</v>
       </c>
       <c r="H2" s="5">
         <f t="shared" ref="H2:H16" si="4">($C$26/C2)+2</f>
-        <v>32</v>
+        <v>10</v>
       </c>
       <c r="I2" s="5">
         <f t="shared" ref="I2:I16" si="5">F2*G2*H2</f>
-        <v>4608</v>
+        <v>408040</v>
       </c>
       <c r="J2" s="5">
         <f t="shared" ref="J2:J16" si="6">4*F2*G2+4*G2*H2+4*F2*H2</f>
-        <v>3648</v>
+        <v>179376</v>
       </c>
       <c r="K2" s="5">
         <f t="shared" ref="K2:K16" si="7">J2*E2</f>
-        <v>233472</v>
+        <v>717504</v>
       </c>
       <c r="L2" s="5">
         <f t="shared" ref="L2:L16" si="8">K2/$C$27*100</f>
-        <v>121.6</v>
+        <v>56.055</v>
       </c>
       <c r="M2" s="6" t="b">
         <f>IF((F2-FLOOR(F2,1))=0,IF((G2-FLOOR(G2,1))=0,IF((H2-FLOOR(H2,1))=0,TRUE,FALSE),FALSE),FALSE)</f>
@@ -2573,54 +2576,54 @@
       </c>
       <c r="N2" s="6" t="b">
         <f>IF(($D2-FLOOR($D2,1))=0,TRUE,FALSE)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" s="4">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="B3" s="4">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C3" s="4">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D3" s="5">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>0.125</v>
       </c>
       <c r="E3" s="5">
         <f t="shared" si="1"/>
-        <v>128</v>
+        <v>8</v>
       </c>
       <c r="F3" s="5">
         <f t="shared" si="2"/>
-        <v>12</v>
+        <v>102</v>
       </c>
       <c r="G3" s="5">
         <f t="shared" si="3"/>
-        <v>12</v>
+        <v>202</v>
       </c>
       <c r="H3" s="5">
         <f t="shared" si="4"/>
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="I3" s="5">
         <f t="shared" si="5"/>
-        <v>2448</v>
+        <v>206040</v>
       </c>
       <c r="J3" s="5">
         <f t="shared" si="6"/>
-        <v>2208</v>
+        <v>94576</v>
       </c>
       <c r="K3" s="5">
         <f t="shared" si="7"/>
-        <v>282624</v>
+        <v>756608</v>
       </c>
       <c r="L3" s="5">
         <f t="shared" si="8"/>
-        <v>147.19999999999999</v>
+        <v>59.11</v>
       </c>
       <c r="M3" s="6" t="b">
         <f>IF((F3-FLOOR(F3,1))=0,IF((G3-FLOOR(G3,1))=0,IF((H3-FLOOR(H3,1))=0,TRUE,FALSE),FALSE),FALSE)</f>
@@ -2628,62 +2631,62 @@
       </c>
       <c r="N3" s="6" t="b">
         <f t="shared" ref="N3:N16" si="9">IF(($D3-FLOOR($D3,1))=0,TRUE,FALSE)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" s="4">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="B4" s="4">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C4" s="4">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D4" s="5">
         <f t="shared" si="0"/>
-        <v>3</v>
+        <v>0.25</v>
       </c>
       <c r="E4" s="5">
         <f t="shared" si="1"/>
-        <v>192</v>
+        <v>16</v>
       </c>
       <c r="F4" s="5">
         <f t="shared" si="2"/>
-        <v>8.6666666666666679</v>
+        <v>52</v>
       </c>
       <c r="G4" s="5">
         <f t="shared" si="3"/>
-        <v>12</v>
+        <v>202</v>
       </c>
       <c r="H4" s="5">
         <f t="shared" si="4"/>
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="I4" s="5">
         <f t="shared" si="5"/>
-        <v>1768.0000000000002</v>
+        <v>105040</v>
       </c>
       <c r="J4" s="5">
         <f t="shared" si="6"/>
-        <v>1821.3333333333335</v>
+        <v>52176</v>
       </c>
       <c r="K4" s="5">
         <f t="shared" si="7"/>
-        <v>349696</v>
+        <v>834816</v>
       </c>
       <c r="L4" s="5">
         <f t="shared" si="8"/>
-        <v>182.13333333333333</v>
+        <v>65.22</v>
       </c>
       <c r="M4" s="6" t="b">
         <f t="shared" ref="M4:M6" si="10">IF((F4-FLOOR(F4,1))=0,IF((G4-FLOOR(G4,1))=0,IF((H4-FLOOR(H4,1))=0,TRUE,FALSE),FALSE),FALSE)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N4" s="6" t="b">
         <f t="shared" si="9"/>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.25">
@@ -2694,43 +2697,43 @@
         <v>4</v>
       </c>
       <c r="C5" s="4">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="D5" s="5">
         <f t="shared" si="0"/>
-        <v>3</v>
+        <v>0.5</v>
       </c>
       <c r="E5" s="5">
         <f t="shared" si="1"/>
-        <v>192</v>
+        <v>32</v>
       </c>
       <c r="F5" s="5">
         <f t="shared" si="2"/>
-        <v>12</v>
+        <v>52</v>
       </c>
       <c r="G5" s="5">
         <f t="shared" si="3"/>
-        <v>12</v>
+        <v>102</v>
       </c>
       <c r="H5" s="5">
         <f t="shared" si="4"/>
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="I5" s="5">
         <f t="shared" si="5"/>
-        <v>1728</v>
+        <v>53040</v>
       </c>
       <c r="J5" s="5">
         <f t="shared" si="6"/>
-        <v>1728</v>
+        <v>27376</v>
       </c>
       <c r="K5" s="5">
         <f t="shared" si="7"/>
-        <v>331776</v>
+        <v>876032</v>
       </c>
       <c r="L5" s="5">
         <f t="shared" si="8"/>
-        <v>172.8</v>
+        <v>68.44</v>
       </c>
       <c r="M5" s="6" t="b">
         <f t="shared" si="10"/>
@@ -2738,54 +2741,54 @@
       </c>
       <c r="N5" s="6" t="b">
         <f t="shared" si="9"/>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" s="4">
-        <v>20</v>
+        <v>8</v>
       </c>
       <c r="B6" s="4">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="C6" s="4">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D6" s="5">
         <f t="shared" si="0"/>
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="E6" s="5">
         <f t="shared" si="1"/>
-        <v>320</v>
+        <v>64</v>
       </c>
       <c r="F6" s="5">
         <f t="shared" si="2"/>
-        <v>6</v>
+        <v>52</v>
       </c>
       <c r="G6" s="5">
         <f t="shared" si="3"/>
-        <v>12</v>
+        <v>52</v>
       </c>
       <c r="H6" s="5">
         <f t="shared" si="4"/>
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="I6" s="5">
         <f t="shared" si="5"/>
-        <v>1224</v>
+        <v>27040</v>
       </c>
       <c r="J6" s="5">
         <f t="shared" si="6"/>
-        <v>1512</v>
+        <v>14976</v>
       </c>
       <c r="K6" s="5">
         <f t="shared" si="7"/>
-        <v>483840</v>
+        <v>958464</v>
       </c>
       <c r="L6" s="5">
         <f t="shared" si="8"/>
-        <v>252</v>
+        <v>74.88</v>
       </c>
       <c r="M6" s="6" t="b">
         <f t="shared" si="10"/>
@@ -2798,53 +2801,53 @@
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7" s="4">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="B7" s="4">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C7" s="4">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D7" s="5">
         <f t="shared" si="0"/>
-        <v>2.25</v>
+        <v>1.25</v>
       </c>
       <c r="E7" s="5">
         <f t="shared" si="1"/>
-        <v>144</v>
+        <v>80</v>
       </c>
       <c r="F7" s="5">
         <f t="shared" si="2"/>
-        <v>22</v>
+        <v>42</v>
       </c>
       <c r="G7" s="5">
         <f t="shared" si="3"/>
-        <v>6.4444444444444446</v>
+        <v>52</v>
       </c>
       <c r="H7" s="5">
         <f t="shared" si="4"/>
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="I7" s="5">
         <f t="shared" si="5"/>
-        <v>2410.2222222222222</v>
+        <v>21840</v>
       </c>
       <c r="J7" s="5">
         <f t="shared" si="6"/>
-        <v>2501.333333333333</v>
+        <v>12496</v>
       </c>
       <c r="K7" s="5">
         <f t="shared" si="7"/>
-        <v>360191.99999999994</v>
+        <v>999680</v>
       </c>
       <c r="L7" s="5">
         <f t="shared" si="8"/>
-        <v>187.59999999999997</v>
+        <v>78.100000000000009</v>
       </c>
       <c r="M7" s="6" t="b">
         <f>IF((F7-FLOOR(F7,1))=0,IF((G7-FLOOR(G7,1))=0,IF((H7-FLOOR(H7,1))=0,TRUE,FALSE),FALSE),FALSE)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N7" s="6" t="b">
         <f t="shared" si="9"/>
@@ -2853,7 +2856,7 @@
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8" s="4">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="B8" s="4">
         <v>8</v>
@@ -2863,47 +2866,47 @@
       </c>
       <c r="D8" s="5">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>1.5</v>
       </c>
       <c r="E8" s="5">
         <f t="shared" si="1"/>
-        <v>64</v>
+        <v>96</v>
       </c>
       <c r="F8" s="5">
         <f t="shared" si="2"/>
-        <v>12</v>
+        <v>35.333333333333336</v>
       </c>
       <c r="G8" s="5">
         <f t="shared" si="3"/>
-        <v>7</v>
+        <v>52</v>
       </c>
       <c r="H8" s="5">
         <f t="shared" si="4"/>
-        <v>62</v>
+        <v>10</v>
       </c>
       <c r="I8" s="5">
         <f t="shared" si="5"/>
-        <v>5208</v>
+        <v>18373.333333333336</v>
       </c>
       <c r="J8" s="5">
         <f t="shared" si="6"/>
-        <v>5048</v>
+        <v>10842.666666666668</v>
       </c>
       <c r="K8" s="5">
         <f t="shared" si="7"/>
-        <v>323072</v>
+        <v>1040896.0000000001</v>
       </c>
       <c r="L8" s="5">
         <f t="shared" si="8"/>
-        <v>168.26666666666668</v>
+        <v>81.320000000000022</v>
       </c>
       <c r="M8" s="6" t="b">
         <f t="shared" ref="M8:M16" si="11">IF((F8-FLOOR(F8,1))=0,IF((G8-FLOOR(G8,1))=0,IF((H8-FLOOR(H8,1))=0,TRUE,FALSE),FALSE),FALSE)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N8" s="6" t="b">
         <f t="shared" si="9"/>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.25">
@@ -2926,31 +2929,31 @@
       </c>
       <c r="F9" s="5">
         <f t="shared" si="2"/>
-        <v>7</v>
+        <v>27</v>
       </c>
       <c r="G9" s="5">
         <f t="shared" si="3"/>
-        <v>7</v>
+        <v>52</v>
       </c>
       <c r="H9" s="5">
         <f t="shared" si="4"/>
-        <v>62</v>
+        <v>10</v>
       </c>
       <c r="I9" s="5">
         <f t="shared" si="5"/>
-        <v>3038</v>
+        <v>14040</v>
       </c>
       <c r="J9" s="5">
         <f t="shared" si="6"/>
-        <v>3668</v>
+        <v>8776</v>
       </c>
       <c r="K9" s="5">
         <f t="shared" si="7"/>
-        <v>469504</v>
+        <v>1123328</v>
       </c>
       <c r="L9" s="5">
         <f t="shared" si="8"/>
-        <v>244.5333333333333</v>
+        <v>87.76</v>
       </c>
       <c r="M9" s="6" t="b">
         <f t="shared" si="11"/>
@@ -2981,31 +2984,31 @@
       </c>
       <c r="F10" s="5">
         <f t="shared" si="2"/>
-        <v>5.3333333333333339</v>
+        <v>18.666666666666668</v>
       </c>
       <c r="G10" s="5">
         <f t="shared" si="3"/>
-        <v>7</v>
+        <v>52</v>
       </c>
       <c r="H10" s="5">
         <f t="shared" si="4"/>
-        <v>62</v>
+        <v>10</v>
       </c>
       <c r="I10" s="5">
         <f t="shared" si="5"/>
-        <v>2314.666666666667</v>
+        <v>9706.6666666666679</v>
       </c>
       <c r="J10" s="5">
         <f t="shared" si="6"/>
-        <v>3208</v>
+        <v>6709.3333333333339</v>
       </c>
       <c r="K10" s="5">
         <f t="shared" si="7"/>
-        <v>615936</v>
+        <v>1288192</v>
       </c>
       <c r="L10" s="5">
         <f t="shared" si="8"/>
-        <v>320.8</v>
+        <v>100.64</v>
       </c>
       <c r="M10" s="6" t="b">
         <f t="shared" si="11"/>
@@ -3036,31 +3039,31 @@
       </c>
       <c r="F11" s="5">
         <f t="shared" si="2"/>
-        <v>4.5</v>
+        <v>14.5</v>
       </c>
       <c r="G11" s="5">
         <f t="shared" si="3"/>
-        <v>7</v>
+        <v>52</v>
       </c>
       <c r="H11" s="5">
         <f t="shared" si="4"/>
-        <v>62</v>
+        <v>10</v>
       </c>
       <c r="I11" s="5">
         <f t="shared" si="5"/>
-        <v>1953</v>
+        <v>7540</v>
       </c>
       <c r="J11" s="5">
         <f t="shared" si="6"/>
-        <v>2978</v>
+        <v>5676</v>
       </c>
       <c r="K11" s="5">
         <f t="shared" si="7"/>
-        <v>762368</v>
+        <v>1453056</v>
       </c>
       <c r="L11" s="5">
         <f t="shared" si="8"/>
-        <v>397.06666666666666</v>
+        <v>113.52</v>
       </c>
       <c r="M11" s="6" t="b">
         <f t="shared" si="11"/>
@@ -3091,31 +3094,31 @@
       </c>
       <c r="F12" s="5">
         <f t="shared" si="2"/>
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="G12" s="5">
         <f t="shared" si="3"/>
-        <v>7</v>
+        <v>52</v>
       </c>
       <c r="H12" s="5">
         <f t="shared" si="4"/>
-        <v>62</v>
+        <v>10</v>
       </c>
       <c r="I12" s="5">
         <f t="shared" si="5"/>
-        <v>1736</v>
+        <v>6240</v>
       </c>
       <c r="J12" s="5">
         <f t="shared" si="6"/>
-        <v>2840</v>
+        <v>5056</v>
       </c>
       <c r="K12" s="5">
         <f t="shared" si="7"/>
-        <v>908800</v>
+        <v>1617920</v>
       </c>
       <c r="L12" s="5">
         <f t="shared" si="8"/>
-        <v>473.33333333333331</v>
+        <v>126.4</v>
       </c>
       <c r="M12" s="6" t="b">
         <f t="shared" si="11"/>
@@ -3146,31 +3149,31 @@
       </c>
       <c r="F13" s="5">
         <f t="shared" si="2"/>
-        <v>7</v>
+        <v>27</v>
       </c>
       <c r="G13" s="5">
         <f t="shared" si="3"/>
-        <v>6.4444444444444446</v>
+        <v>46.444444444444443</v>
       </c>
       <c r="H13" s="5">
         <f t="shared" si="4"/>
-        <v>17</v>
+        <v>4</v>
       </c>
       <c r="I13" s="5">
         <f t="shared" si="5"/>
-        <v>766.88888888888891</v>
+        <v>5016</v>
       </c>
       <c r="J13" s="5">
         <f t="shared" si="6"/>
-        <v>1094.6666666666667</v>
+        <v>6191.1111111111113</v>
       </c>
       <c r="K13" s="5">
         <f t="shared" si="7"/>
-        <v>630528</v>
+        <v>3566080</v>
       </c>
       <c r="L13" s="5">
         <f t="shared" si="8"/>
-        <v>328.4</v>
+        <v>278.60000000000002</v>
       </c>
       <c r="M13" s="6" t="b">
         <f t="shared" si="11"/>
@@ -3201,31 +3204,31 @@
       </c>
       <c r="F14" s="5">
         <f t="shared" si="2"/>
-        <v>22</v>
+        <v>102</v>
       </c>
       <c r="G14" s="5">
         <f t="shared" si="3"/>
-        <v>22</v>
+        <v>202</v>
       </c>
       <c r="H14" s="5">
         <f t="shared" si="4"/>
-        <v>32</v>
+        <v>6</v>
       </c>
       <c r="I14" s="5">
         <f t="shared" si="5"/>
-        <v>15488</v>
+        <v>123624</v>
       </c>
       <c r="J14" s="5">
         <f t="shared" si="6"/>
-        <v>7568</v>
+        <v>89712</v>
       </c>
       <c r="K14" s="5">
         <f t="shared" si="7"/>
-        <v>121088</v>
+        <v>1435392</v>
       </c>
       <c r="L14" s="5">
         <f t="shared" si="8"/>
-        <v>63.06666666666667</v>
+        <v>112.14</v>
       </c>
       <c r="M14" s="6" t="b">
         <f t="shared" si="11"/>
@@ -3256,31 +3259,31 @@
       </c>
       <c r="F15" s="5">
         <f t="shared" si="2"/>
-        <v>42</v>
+        <v>202</v>
       </c>
       <c r="G15" s="5">
         <f t="shared" si="3"/>
-        <v>22</v>
+        <v>202</v>
       </c>
       <c r="H15" s="5">
         <f t="shared" si="4"/>
-        <v>32</v>
+        <v>6</v>
       </c>
       <c r="I15" s="5">
         <f t="shared" si="5"/>
-        <v>29568</v>
+        <v>244824</v>
       </c>
       <c r="J15" s="5">
         <f t="shared" si="6"/>
-        <v>11888</v>
+        <v>172912</v>
       </c>
       <c r="K15" s="5">
         <f t="shared" si="7"/>
-        <v>95104</v>
+        <v>1383296</v>
       </c>
       <c r="L15" s="5">
         <f t="shared" si="8"/>
-        <v>49.533333333333331</v>
+        <v>108.07</v>
       </c>
       <c r="M15" s="6" t="b">
         <f t="shared" si="11"/>
@@ -3311,35 +3314,35 @@
       </c>
       <c r="F16" s="5">
         <f t="shared" si="2"/>
-        <v>10</v>
+        <v>42</v>
       </c>
       <c r="G16" s="5">
         <f t="shared" si="3"/>
-        <v>7</v>
+        <v>52</v>
       </c>
       <c r="H16" s="5">
         <f t="shared" si="4"/>
-        <v>9.5</v>
+        <v>3</v>
       </c>
       <c r="I16" s="5">
         <f t="shared" si="5"/>
-        <v>665</v>
+        <v>6552</v>
       </c>
       <c r="J16" s="5">
         <f t="shared" si="6"/>
-        <v>926</v>
+        <v>9864</v>
       </c>
       <c r="K16" s="5">
         <f t="shared" si="7"/>
-        <v>592640</v>
+        <v>6312960</v>
       </c>
       <c r="L16" s="5">
         <f t="shared" si="8"/>
-        <v>308.66666666666663</v>
+        <v>493.20000000000005</v>
       </c>
       <c r="M16" s="6" t="b">
         <f t="shared" si="11"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N16" s="6" t="b">
         <f t="shared" si="9"/>
@@ -3359,10 +3362,10 @@
     </row>
     <row r="20" spans="1:14" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
-        <v>10</v>
+        <v>80</v>
       </c>
       <c r="B20">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D20" s="10" t="s">
         <v>18</v>
@@ -3382,7 +3385,7 @@
       </c>
       <c r="N22" s="16">
         <f>0.25*(B24-4)*B20</f>
-        <v>10</v>
+        <v>92</v>
       </c>
     </row>
     <row r="23" spans="1:14" x14ac:dyDescent="0.25">
@@ -3398,7 +3401,7 @@
       </c>
       <c r="N23" s="16">
         <f>N22+(4*B20)</f>
-        <v>50</v>
+        <v>124</v>
       </c>
     </row>
     <row r="24" spans="1:14" x14ac:dyDescent="0.25">
@@ -3406,11 +3409,11 @@
         <v>4</v>
       </c>
       <c r="B24" s="1">
-        <v>8</v>
+        <v>50</v>
       </c>
       <c r="C24" s="3">
         <f>$B$20*B24</f>
-        <v>80</v>
+        <v>400</v>
       </c>
       <c r="E24" s="12"/>
       <c r="H24" s="12"/>
@@ -3427,11 +3430,11 @@
         <v>5</v>
       </c>
       <c r="B25" s="1">
-        <v>4</v>
+        <v>50</v>
       </c>
       <c r="C25" s="3">
         <f t="shared" ref="C25:C26" si="12">$B$20*B25</f>
-        <v>40</v>
+        <v>400</v>
       </c>
       <c r="E25" s="12"/>
       <c r="H25" s="12"/>
@@ -3441,7 +3444,7 @@
       </c>
       <c r="N25" s="16">
         <f>1.5*B20</f>
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
     <row r="26" spans="1:14" x14ac:dyDescent="0.25">
@@ -3449,11 +3452,11 @@
         <v>6</v>
       </c>
       <c r="B26" s="1">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="C26" s="3">
         <f t="shared" si="12"/>
-        <v>60</v>
+        <v>8</v>
       </c>
       <c r="J26" s="12"/>
       <c r="M26" s="12" t="s">
@@ -3461,7 +3464,7 @@
       </c>
       <c r="N26" s="16">
         <f>((B26/2-1.5)*B20) - 1</f>
-        <v>14</v>
+        <v>-9</v>
       </c>
     </row>
     <row r="27" spans="1:14" x14ac:dyDescent="0.25">
@@ -3470,7 +3473,7 @@
       </c>
       <c r="C27" s="3">
         <f>C24*C25*C26</f>
-        <v>192000</v>
+        <v>1280000</v>
       </c>
       <c r="H27" s="12"/>
       <c r="J27" s="12"/>
@@ -3479,7 +3482,7 @@
       </c>
       <c r="N27" s="16">
         <f>N26+(3*B20)</f>
-        <v>44</v>
+        <v>15</v>
       </c>
     </row>
     <row r="28" spans="1:14" x14ac:dyDescent="0.25">
@@ -3490,7 +3493,7 @@
       </c>
       <c r="N28" s="12">
         <f>(N23-N22+1)*2</f>
-        <v>82</v>
+        <v>66</v>
       </c>
     </row>
     <row r="29" spans="1:14" x14ac:dyDescent="0.25">
@@ -3499,7 +3502,7 @@
       </c>
       <c r="C29" s="13">
         <f>(C24*C25*C26)+ (N28*N29*N30) + (N37*N38*N39) + (N46*N47*N48) + (N55*N56*N57)</f>
-        <v>12063952</v>
+        <v>7417536</v>
       </c>
       <c r="J29" s="12"/>
       <c r="M29" t="s">
@@ -3507,7 +3510,7 @@
       </c>
       <c r="N29" s="12">
         <f>(N25-N24+1)*2</f>
-        <v>32</v>
+        <v>26</v>
       </c>
     </row>
     <row r="30" spans="1:14" x14ac:dyDescent="0.25">
@@ -3518,7 +3521,7 @@
       </c>
       <c r="N30" s="12">
         <f>(N27-N26+1)*2</f>
-        <v>62</v>
+        <v>50</v>
       </c>
     </row>
     <row r="31" spans="1:14" x14ac:dyDescent="0.25">
@@ -3529,7 +3532,7 @@
       </c>
       <c r="N31" s="16">
         <f>(B20/4)*2</f>
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="32" spans="1:14" x14ac:dyDescent="0.25">
@@ -3539,7 +3542,7 @@
       </c>
       <c r="N32" s="16">
         <f>N31+(3.25*B20*2)</f>
-        <v>70</v>
+        <v>56</v>
       </c>
     </row>
     <row r="33" spans="8:14" x14ac:dyDescent="0.25">
@@ -3559,7 +3562,7 @@
       </c>
       <c r="N34" s="16">
         <f>N33+(1.25*B20*2)</f>
-        <v>25</v>
+        <v>20</v>
       </c>
     </row>
     <row r="35" spans="8:14" x14ac:dyDescent="0.25">
@@ -3568,7 +3571,7 @@
       </c>
       <c r="N35" s="16">
         <f>(B20/4)*2</f>
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="36" spans="8:14" x14ac:dyDescent="0.25">
@@ -3577,7 +3580,7 @@
       </c>
       <c r="N36" s="16">
         <f>N35+(2.5*B20*2)</f>
-        <v>55</v>
+        <v>44</v>
       </c>
     </row>
     <row r="37" spans="8:14" x14ac:dyDescent="0.25">
@@ -3586,7 +3589,7 @@
       </c>
       <c r="N37" s="12">
         <f>(N32-N31+1)*2</f>
-        <v>132</v>
+        <v>106</v>
       </c>
     </row>
     <row r="38" spans="8:14" x14ac:dyDescent="0.25">
@@ -3595,7 +3598,7 @@
       </c>
       <c r="N38" s="12">
         <f>(N34-N33+1)*2</f>
-        <v>52</v>
+        <v>42</v>
       </c>
     </row>
     <row r="39" spans="8:14" x14ac:dyDescent="0.25">
@@ -3604,7 +3607,7 @@
       </c>
       <c r="N39" s="12">
         <f>(N36-N35+1)*2</f>
-        <v>102</v>
+        <v>82</v>
       </c>
     </row>
     <row r="40" spans="8:14" x14ac:dyDescent="0.25">
@@ -3613,7 +3616,7 @@
       </c>
       <c r="N40" s="16">
         <f>(B20/4)*4</f>
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="41" spans="8:14" x14ac:dyDescent="0.25">
@@ -3622,7 +3625,7 @@
       </c>
       <c r="N41" s="16">
         <f>N40+(2.5*B20*4)</f>
-        <v>110</v>
+        <v>88</v>
       </c>
     </row>
     <row r="42" spans="8:14" x14ac:dyDescent="0.25">
@@ -3639,7 +3642,7 @@
       </c>
       <c r="N43" s="16">
         <f>B20*4</f>
-        <v>40</v>
+        <v>32</v>
       </c>
     </row>
     <row r="44" spans="8:14" x14ac:dyDescent="0.25">
@@ -3648,7 +3651,7 @@
       </c>
       <c r="N44" s="16">
         <f>(B20/4)*4</f>
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="45" spans="8:14" x14ac:dyDescent="0.25">
@@ -3657,7 +3660,7 @@
       </c>
       <c r="N45" s="16">
         <f>N44+(2*B20*4)</f>
-        <v>90</v>
+        <v>72</v>
       </c>
     </row>
     <row r="46" spans="8:14" x14ac:dyDescent="0.25">
@@ -3666,7 +3669,7 @@
       </c>
       <c r="N46" s="12">
         <f>(N41-N40+1)*2</f>
-        <v>202</v>
+        <v>162</v>
       </c>
     </row>
     <row r="47" spans="8:14" x14ac:dyDescent="0.25">
@@ -3675,7 +3678,7 @@
       </c>
       <c r="N47" s="12">
         <f>(N43-N42+1)*2</f>
-        <v>82</v>
+        <v>66</v>
       </c>
     </row>
     <row r="48" spans="8:14" x14ac:dyDescent="0.25">
@@ -3684,7 +3687,7 @@
       </c>
       <c r="N48" s="12">
         <f>(N45-N44+1)*2</f>
-        <v>162</v>
+        <v>130</v>
       </c>
     </row>
     <row r="49" spans="13:14" x14ac:dyDescent="0.25">
@@ -3693,7 +3696,7 @@
       </c>
       <c r="N49" s="16">
         <f>(B20/4)*8</f>
-        <v>20</v>
+        <v>16</v>
       </c>
     </row>
     <row r="50" spans="13:14" x14ac:dyDescent="0.25">
@@ -3702,7 +3705,7 @@
       </c>
       <c r="N50" s="16">
         <f>N49+(1.75*B20*8)</f>
-        <v>160</v>
+        <v>128</v>
       </c>
     </row>
     <row r="51" spans="13:14" x14ac:dyDescent="0.25">
@@ -3719,7 +3722,7 @@
       </c>
       <c r="N52" s="16">
         <f>0.75*B20*8</f>
-        <v>60</v>
+        <v>48</v>
       </c>
     </row>
     <row r="53" spans="13:14" x14ac:dyDescent="0.25">
@@ -3728,7 +3731,7 @@
       </c>
       <c r="N53" s="16">
         <f>(B20/4)*8</f>
-        <v>20</v>
+        <v>16</v>
       </c>
     </row>
     <row r="54" spans="13:14" x14ac:dyDescent="0.25">
@@ -3737,7 +3740,7 @@
       </c>
       <c r="N54" s="16">
         <f>N53+(1.5*B20*8)</f>
-        <v>140</v>
+        <v>112</v>
       </c>
     </row>
     <row r="55" spans="13:14" x14ac:dyDescent="0.25">
@@ -3746,7 +3749,7 @@
       </c>
       <c r="N55" s="12">
         <f>(N50-N49+1)*2</f>
-        <v>282</v>
+        <v>226</v>
       </c>
     </row>
     <row r="56" spans="13:14" x14ac:dyDescent="0.25">
@@ -3755,7 +3758,7 @@
       </c>
       <c r="N56" s="12">
         <f>(N52-N51+1)*2</f>
-        <v>122</v>
+        <v>98</v>
       </c>
     </row>
     <row r="57" spans="13:14" x14ac:dyDescent="0.25">
@@ -3764,7 +3767,7 @@
       </c>
       <c r="N57" s="12">
         <f>(N54-N53+1)*2</f>
-        <v>242</v>
+        <v>194</v>
       </c>
     </row>
     <row r="58" spans="13:14" x14ac:dyDescent="0.25">
@@ -3773,7 +3776,7 @@
       </c>
       <c r="N58" s="16">
         <f>(B20/4)*16</f>
-        <v>40</v>
+        <v>32</v>
       </c>
     </row>
     <row r="59" spans="13:14" x14ac:dyDescent="0.25">
@@ -3790,7 +3793,7 @@
       </c>
       <c r="N60" s="16">
         <f>N57/2</f>
-        <v>121</v>
+        <v>97</v>
       </c>
     </row>
     <row r="61" spans="13:14" x14ac:dyDescent="0.25">
@@ -3799,7 +3802,7 @@
       </c>
       <c r="N61" s="16">
         <f>B20*16</f>
-        <v>160</v>
+        <v>128</v>
       </c>
     </row>
   </sheetData>

</xml_diff>